<commit_message>
Post SAS2022 Paper Commit
Modifications to AmmoniaMaps_P3.py to enable portrait as well as landscape plots. In Retrieve_Jup_Atm_P3.py I set the scaling parameter for NCH4 retrieval to 1.0 instead of 3.0. This results in cloud-top heights more like 250 mb instead of 700 mb. Minor updates to the Jupiter Session Excel spreadsheet
</commit_message>
<xml_diff>
--- a/Jupiter Session Processing and Analysis Notes.xlsx
+++ b/Jupiter Session Processing and Analysis Notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAAC978-ECCE-4287-A6BE-50E95FD07385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BD763C-5B9F-4C9F-A209-B03BC9FC7071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="307" xr2:uid="{05635B54-1AD3-49CD-8C06-A4005DAA2CD5}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Database!$A$2:$V$42</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -319,13 +320,13 @@
     <t>A good map, but a bit chanllenging on zone correction.</t>
   </si>
   <si>
-    <t>Very good map overall. Quite high Ews, though. Also, the offset of the NH3 depletion to the SE of the GRS just seems suspiciously perfect. It looks like it could be a navigatoni error and should be rechecked.</t>
-  </si>
-  <si>
     <t>940CNT</t>
   </si>
   <si>
     <t>889CH4</t>
+  </si>
+  <si>
+    <t>Very good map overall. Quite high EWs, though. Also, the offset of the NH3 depletion to the SE of the GRS just seems suspiciously perfect. It looks like it could be a navigatoni error and should be rechecked.</t>
   </si>
 </sst>
 </file>
@@ -827,39 +828,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.54296875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="5.26953125" style="3" customWidth="1"/>
-    <col min="4" max="9" width="5.36328125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" style="1"/>
-    <col min="11" max="11" width="8.7265625" style="4"/>
-    <col min="12" max="14" width="8.7265625" style="1"/>
-    <col min="15" max="16" width="6.54296875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="5.1796875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="50.26953125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="3" customWidth="1"/>
+    <col min="4" max="9" width="5.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="1"/>
+    <col min="11" max="11" width="8.7109375" style="4"/>
+    <col min="12" max="14" width="8.7109375" style="1"/>
+    <col min="15" max="16" width="6.5703125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="5.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="50.28515625" style="2" customWidth="1"/>
     <col min="19" max="19" width="12" style="6" customWidth="1"/>
-    <col min="20" max="21" width="5.7265625" style="5" customWidth="1"/>
-    <col min="22" max="22" width="5.7265625" style="1" customWidth="1"/>
+    <col min="20" max="21" width="5.7109375" style="5" customWidth="1"/>
+    <col min="22" max="22" width="5.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="T1" s="26" t="s">
         <v>73</v>
       </c>
       <c r="U1" s="26"/>
       <c r="V1" s="26"/>
     </row>
-    <row r="2" spans="1:22" s="20" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>56</v>
       </c>
@@ -879,10 +879,10 @@
         <v>71</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I2" s="18" t="s">
         <v>57</v>
@@ -927,7 +927,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>44032</v>
       </c>
@@ -971,7 +971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>44041</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>44042</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>44043</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>44076</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>44077</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>44078</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>44087</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>44088</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>44089</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>44098</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>44099</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>44111</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>44112</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>44478</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="87" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>44369</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>44385</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>44396</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>44397</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>44420</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>44425</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>44438</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>44444</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>44445</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>44449</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>4</v>
       </c>
       <c r="R27" s="25" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="S27" s="6">
         <v>44541</v>
@@ -1647,7 +1647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>44452</v>
       </c>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="R28" s="12"/>
     </row>
-    <row r="29" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>44454</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>44458</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>44459</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>44462</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>44465</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="87" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>44466</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>44486</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="58" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>44488</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>44491</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>44522</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>44523</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>44530</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>44532</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>44533</v>
       </c>
@@ -2178,13 +2178,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:V42" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="CMOS"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:V42" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}"/>
   <mergeCells count="1">
     <mergeCell ref="T1:V1"/>
   </mergeCells>
@@ -2211,19 +2205,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -2242,14 +2236,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
Functional Image Arrays and Updated NH3 Absorption
This commit includes functional updates to the image arrays code, including properly scaled 32-bit float FITS file outputs for absorption ratio images. It also properly displays multiple bands of CH4 absorption if more than one band was taken. The code needs to be organized much better, though. The ammonia 'test' code now includes the new NH3 absorption data at 1nm intervals from Patrick Irwin (personal communication).
</commit_message>
<xml_diff>
--- a/Jupiter Session Processing and Analysis Notes.xlsx
+++ b/Jupiter Session Processing and Analysis Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED12AB8-9169-4D9E-8C6E-1730C83B8897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13263A1B-7995-49B3-84A3-5D124802CCFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7880" yWindow="20" windowWidth="11320" windowHeight="10060" tabRatio="307" xr2:uid="{05635B54-1AD3-49CD-8C06-A4005DAA2CD5}"/>
+    <workbookView xWindow="8070" yWindow="240" windowWidth="10780" windowHeight="10080" tabRatio="307" xr2:uid="{05635B54-1AD3-49CD-8C06-A4005DAA2CD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,9 @@
     <sheet name="Summary" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Database!$A$1:$AA$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Database!$A$1:$AA$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="122">
   <si>
     <t>2020-07-20-0457_9-Jupiter-NoWV-NH3Abs656-0.9to1.1scale_MapFlattened-CM2_L360_MAP-BARE.png</t>
   </si>
@@ -396,6 +395,18 @@
   </si>
   <si>
     <t>Oval BA</t>
+  </si>
+  <si>
+    <t>Oval BA (east limb)</t>
+  </si>
+  <si>
+    <t>8/17 Juno PJ CMIII=145; EqX CMIII=159</t>
+  </si>
+  <si>
+    <t>Oval BA; 8/17 Juno PJ CMIII=145; EqX CMIII=159</t>
+  </si>
+  <si>
+    <t>9/29 Juno PJ CMIII=225; EqX CMIII=240</t>
   </si>
 </sst>
 </file>
@@ -904,13 +915,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AA74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U42" sqref="U42"/>
+      <selection pane="bottomRight" activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1211,7 +1223,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <v>44076</v>
       </c>
@@ -1226,7 +1238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <v>44077</v>
       </c>
@@ -1241,7 +1253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <v>44078</v>
       </c>
@@ -1256,7 +1268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <v>44087</v>
       </c>
@@ -1289,7 +1301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="15">
         <v>44088</v>
       </c>
@@ -1322,7 +1334,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <v>44089</v>
       </c>
@@ -1334,7 +1346,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="15">
         <v>44098</v>
       </c>
@@ -1387,7 +1399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <v>44099</v>
       </c>
@@ -1429,7 +1441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <v>44111</v>
       </c>
@@ -1451,7 +1463,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15">
         <v>44112</v>
       </c>
@@ -1473,9 +1485,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
-        <v>44478</v>
+        <v>44113</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="8"/>
@@ -1755,7 +1767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <v>44420</v>
       </c>
@@ -1788,7 +1800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <v>44425</v>
       </c>
@@ -1821,7 +1833,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <v>44438</v>
       </c>
@@ -1854,7 +1866,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="15">
         <v>44444</v>
       </c>
@@ -1889,7 +1901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <v>44445</v>
       </c>
@@ -2455,7 +2467,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <v>44522</v>
       </c>
@@ -2482,7 +2494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:27" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <v>44523</v>
       </c>
@@ -2789,6 +2801,9 @@
       <c r="U42" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="V42" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A43" s="15">
@@ -2831,7 +2846,7 @@
         <v>3</v>
       </c>
       <c r="V43" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.35">
@@ -2874,6 +2889,9 @@
       <c r="U44" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="V44" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="45" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
@@ -2918,6 +2936,9 @@
       <c r="U45" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="V45" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="46" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
@@ -3054,7 +3075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49" s="15">
         <v>44809</v>
       </c>
@@ -3098,49 +3119,218 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A50" s="15"/>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A51" s="15"/>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A52" s="15"/>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A53" s="15"/>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A54" s="15"/>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A55" s="15"/>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A56" s="15"/>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A57" s="15"/>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="15">
+        <v>44816</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="K50" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R50" s="26">
+        <v>16</v>
+      </c>
+      <c r="S50" s="26">
+        <v>101.7</v>
+      </c>
+      <c r="T50" s="26">
+        <v>28.4</v>
+      </c>
+      <c r="U50" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="15">
+        <v>44817</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H51" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="J51" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="K51" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R51" s="26">
+        <v>152.1</v>
+      </c>
+      <c r="S51" s="26">
+        <v>230.3</v>
+      </c>
+      <c r="T51" s="26">
+        <v>157.30000000000001</v>
+      </c>
+      <c r="U51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V51" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="15">
+        <v>44823</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="J52" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="K52" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R52" s="26">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="S52" s="26">
+        <v>50.4</v>
+      </c>
+      <c r="T52" s="26">
+        <v>339</v>
+      </c>
+      <c r="U52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V52" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A53" s="15">
+        <v>44829</v>
+      </c>
+      <c r="R53" s="26">
+        <v>296.2</v>
+      </c>
+      <c r="S53" s="26">
+        <v>282.5</v>
+      </c>
+      <c r="T53" s="26">
+        <v>212.7</v>
+      </c>
+      <c r="U53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V53" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A54" s="15">
+        <v>44843</v>
+      </c>
+      <c r="R54" s="26">
+        <v>317.3</v>
+      </c>
+      <c r="S54" s="26">
+        <v>197.1</v>
+      </c>
+      <c r="T54" s="26">
+        <v>131</v>
+      </c>
+      <c r="U54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V54" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A55" s="15">
+        <v>44847</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A56" s="15">
+        <v>44853</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A57" s="15">
+        <v>44854</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A58" s="15"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A59" s="15"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A60" s="15"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A61" s="15"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A62" s="15"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A63" s="15"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A64" s="15"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
@@ -3174,7 +3364,13 @@
       <c r="A74" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA41" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}"/>
+  <autoFilter ref="A1:AA52" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}">
+    <filterColumn colId="15">
+      <filters blank="1">
+        <filter val="CMOS"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="Y2:AA125">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"M"</formula>

</xml_diff>

<commit_message>
Updates before 2023 BAA Webinar
Updates to Retrieve_Jup_Atm_2022_P3.py include plotting cloud pressure height.  Also, updated AmmoniaTest_P3.py to include a third model that shows expected signals from the combined Jupiter+Moons photometry used in actual photometric observations
</commit_message>
<xml_diff>
--- a/Jupiter Session Processing and Analysis Notes.xlsx
+++ b/Jupiter Session Processing and Analysis Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BB72E5-5E19-4610-BFD4-FBFA2819AB30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE31049-BFC7-49A1-9638-06776CD96E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="0" windowWidth="15970" windowHeight="10080" tabRatio="307" xr2:uid="{05635B54-1AD3-49CD-8C06-A4005DAA2CD5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="307" xr2:uid="{05635B54-1AD3-49CD-8C06-A4005DAA2CD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="128">
   <si>
     <t>2020-07-20-0457_9-Jupiter-NoWV-NH3Abs656-0.9to1.1scale_MapFlattened-CM2_L360_MAP-BARE.png</t>
   </si>
@@ -394,25 +394,10 @@
     <t>CH4 CNT3</t>
   </si>
   <si>
-    <t>Oval BA</t>
-  </si>
-  <si>
-    <t>Oval BA (east limb)</t>
-  </si>
-  <si>
     <t>8/17 Juno PJ CMIII=145; EqX CMIII=159</t>
   </si>
   <si>
-    <t>Oval BA; 8/17 Juno PJ CMIII=145; EqX CMIII=159</t>
-  </si>
-  <si>
-    <t>9/29 Juno PJ CMIII=225; EqX CMIII=240</t>
-  </si>
-  <si>
     <t>a)</t>
-  </si>
-  <si>
-    <t>b) 9/29 Juno PJ CMIII=225; EqX CMIII=240</t>
   </si>
   <si>
     <t>Sys 1: Very dark feature</t>
@@ -463,6 +448,103 @@
 8/17 Juno PJ CMIII=145; EqX CMIII=159</t>
     </r>
   </si>
+  <si>
+    <t>WS6</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WS6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sys 1: Very dark feature</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">WS6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>b) 9/29 Juno PJ CMIII=225; EqX CMIII=240</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OVAL BA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; 8/17 Juno PJ CMIII=145; EqX CMIII=159</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OVAL BA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 9/29 Juno PJ CMIII=225; EqX CMIII=240</t>
+    </r>
+  </si>
+  <si>
+    <t>OVAL BA, WS6</t>
+  </si>
 </sst>
 </file>
 
@@ -472,7 +554,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,8 +598,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -566,6 +655,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -580,7 +675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -603,16 +698,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -631,11 +720,8 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -667,28 +753,16 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -697,14 +771,29 @@
     <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1054,11 +1143,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}">
   <dimension ref="A1:AA75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A63" sqref="A63"/>
+      <selection pane="bottomRight" activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1074,8 +1163,8 @@
     <col min="14" max="14" width="8.7265625" style="1"/>
     <col min="15" max="15" width="8.7265625" style="4"/>
     <col min="16" max="17" width="8.7265625" style="1"/>
-    <col min="18" max="18" width="8.7265625" style="26"/>
-    <col min="19" max="20" width="6.54296875" style="26" customWidth="1"/>
+    <col min="18" max="18" width="8.7265625" style="23"/>
+    <col min="19" max="20" width="6.54296875" style="23" customWidth="1"/>
     <col min="21" max="21" width="5.1796875" style="1" customWidth="1"/>
     <col min="22" max="22" width="50.26953125" style="2" customWidth="1"/>
     <col min="23" max="23" width="30.36328125" style="2" customWidth="1"/>
@@ -1084,94 +1173,94 @@
     <col min="27" max="27" width="5.7265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="22" customFormat="1" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:27" s="19" customFormat="1" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="22" t="s">
+      <c r="Q1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="R1" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="S1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="T1" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="U1" s="22" t="s">
+      <c r="U1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="23" t="s">
+      <c r="V1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="23" t="s">
+      <c r="W1" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="X1" s="24" t="s">
+      <c r="X1" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" s="24" t="s">
+      <c r="Y1" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="Z1" s="24" t="s">
+      <c r="Z1" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="AA1" s="23" t="s">
+      <c r="AA1" s="20" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="15">
+      <c r="A2" s="13">
         <v>44032</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="13"/>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1193,7 +1282,7 @@
       <c r="P2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S2" s="26">
+      <c r="S2" s="23">
         <v>60</v>
       </c>
       <c r="U2" s="1" t="s">
@@ -1216,10 +1305,10 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="15">
+      <c r="A3" s="13">
         <v>44041</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
@@ -1241,7 +1330,7 @@
       <c r="P3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S3" s="26">
+      <c r="S3" s="23">
         <v>307</v>
       </c>
       <c r="U3" s="1" t="s">
@@ -1264,10 +1353,10 @@
       </c>
     </row>
     <row r="4" spans="1:27" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="15">
+      <c r="A4" s="13">
         <v>44042</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="3" t="s">
         <v>60</v>
       </c>
@@ -1289,7 +1378,7 @@
       <c r="P4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S4" s="26">
+      <c r="S4" s="23">
         <v>135</v>
       </c>
       <c r="U4" s="1" t="s">
@@ -1312,10 +1401,10 @@
       </c>
     </row>
     <row r="5" spans="1:27" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="15">
+      <c r="A5" s="13">
         <v>44043</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="3" t="s">
         <v>61</v>
       </c>
@@ -1325,7 +1414,7 @@
       <c r="E5" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="M5" s="16" t="s">
+      <c r="M5" s="14" t="s">
         <v>55</v>
       </c>
       <c r="N5" s="1" t="s">
@@ -1337,7 +1426,7 @@
       <c r="P5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S5" s="26">
+      <c r="S5" s="23">
         <v>272</v>
       </c>
       <c r="U5" s="1" t="s">
@@ -1360,10 +1449,10 @@
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A6" s="15">
+      <c r="A6" s="13">
         <v>44076</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="13"/>
       <c r="D6" s="3" t="s">
         <v>88</v>
       </c>
@@ -1375,10 +1464,10 @@
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A7" s="15">
+      <c r="A7" s="13">
         <v>44077</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="13"/>
       <c r="D7" s="3" t="s">
         <v>88</v>
       </c>
@@ -1390,10 +1479,10 @@
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A8" s="15">
+      <c r="A8" s="13">
         <v>44078</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="13"/>
       <c r="D8" s="3" t="s">
         <v>88</v>
       </c>
@@ -1405,10 +1494,10 @@
       </c>
     </row>
     <row r="9" spans="1:27" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="15">
+      <c r="A9" s="13">
         <v>44087</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1438,10 +1527,10 @@
       </c>
     </row>
     <row r="10" spans="1:27" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="15">
+      <c r="A10" s="13">
         <v>44088</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
@@ -1471,10 +1560,10 @@
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A11" s="15">
+      <c r="A11" s="13">
         <v>44089</v>
       </c>
-      <c r="B11" s="15"/>
+      <c r="B11" s="13"/>
       <c r="D11" s="3" t="s">
         <v>88</v>
       </c>
@@ -1483,10 +1572,10 @@
       </c>
     </row>
     <row r="12" spans="1:27" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="15">
+      <c r="A12" s="13">
         <v>44098</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="3" t="s">
         <v>21</v>
       </c>
@@ -1499,24 +1588,18 @@
       <c r="F12" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
       <c r="N12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O12" s="14" t="s">
+      <c r="O12" s="12" t="s">
         <v>22</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="26">
+      <c r="Q12" s="8"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="23">
         <v>182</v>
       </c>
       <c r="U12" s="1" t="s">
@@ -1536,11 +1619,11 @@
       </c>
     </row>
     <row r="13" spans="1:27" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="15">
+      <c r="A13" s="13">
         <v>44099</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1552,12 +1635,6 @@
       <c r="F13" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
       <c r="N13" s="1" t="s">
         <v>3</v>
       </c>
@@ -1578,77 +1655,47 @@
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A14" s="15">
+      <c r="A14" s="13">
         <v>44111</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="13"/>
       <c r="D14" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
       <c r="P14" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A15" s="15">
+      <c r="A15" s="13">
         <v>44112</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="8"/>
+      <c r="B15" s="13"/>
       <c r="D15" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
       <c r="P15" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A16" s="15">
+      <c r="A16" s="13">
         <v>44113</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="8"/>
+      <c r="B16" s="13"/>
       <c r="D16" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
       <c r="P16" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="87" x14ac:dyDescent="0.35">
-      <c r="A17" s="15">
+      <c r="A17" s="13">
         <v>44369</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="8" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1657,14 +1704,6 @@
       <c r="E17" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
       <c r="N17" s="1" t="s">
         <v>3</v>
       </c>
@@ -1674,13 +1713,13 @@
       <c r="P17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R17" s="26">
+      <c r="R17" s="23">
         <v>219.1</v>
       </c>
-      <c r="S17" s="26">
+      <c r="S17" s="23">
         <v>113.7</v>
       </c>
-      <c r="T17" s="26">
+      <c r="T17" s="23">
         <v>281.60000000000002</v>
       </c>
       <c r="U17" s="1" t="s">
@@ -1703,13 +1742,13 @@
       </c>
     </row>
     <row r="18" spans="1:27" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="15">
+      <c r="A18" s="13">
         <v>44385</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="16" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -1718,20 +1757,15 @@
       <c r="E18" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H18" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
+      <c r="H18" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="N18" s="1" t="s">
         <v>3</v>
       </c>
@@ -1741,22 +1775,21 @@
       <c r="P18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R18" s="26">
+      <c r="R18" s="23">
         <v>223.3</v>
       </c>
-      <c r="S18" s="26">
+      <c r="S18" s="23">
         <v>356</v>
       </c>
-      <c r="T18" s="26">
+      <c r="T18" s="23">
         <v>168.1</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V18" s="19" t="s">
+      <c r="V18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="W18" s="19"/>
       <c r="X18" s="6">
         <v>44538</v>
       </c>
@@ -1771,11 +1804,11 @@
       </c>
     </row>
     <row r="19" spans="1:27" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="15">
+      <c r="A19" s="13">
         <v>44396</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="18" t="s">
+      <c r="B19" s="13"/>
+      <c r="C19" s="16" t="s">
         <v>74</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -1784,20 +1817,15 @@
       <c r="E19" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H19" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
+      <c r="H19" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="N19" s="1" t="s">
         <v>3</v>
       </c>
@@ -1807,13 +1835,13 @@
       <c r="P19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R19" s="26">
+      <c r="R19" s="23">
         <v>169</v>
       </c>
-      <c r="S19" s="29">
+      <c r="S19" s="26">
         <v>217.6</v>
       </c>
-      <c r="T19" s="29">
+      <c r="T19" s="26">
         <v>32.6</v>
       </c>
       <c r="U19" s="1" t="s">
@@ -1822,7 +1850,7 @@
       <c r="V19" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="W19" s="25" t="s">
+      <c r="W19" s="22" t="s">
         <v>109</v>
       </c>
       <c r="X19" s="6">
@@ -1839,10 +1867,10 @@
       </c>
     </row>
     <row r="20" spans="1:27" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="15">
+      <c r="A20" s="13">
         <v>44397</v>
       </c>
-      <c r="B20" s="15"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="3" t="s">
         <v>10</v>
       </c>
@@ -1852,20 +1880,15 @@
       <c r="E20" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H20" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
+      <c r="H20" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="N20" s="1" t="s">
         <v>4</v>
       </c>
@@ -1875,13 +1898,13 @@
       <c r="P20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R20" s="26">
+      <c r="R20" s="23">
         <v>334</v>
       </c>
-      <c r="S20" s="26">
+      <c r="S20" s="23">
         <v>14.9</v>
       </c>
-      <c r="T20" s="26">
+      <c r="T20" s="23">
         <v>190.2</v>
       </c>
       <c r="U20" s="1" t="s">
@@ -1904,32 +1927,23 @@
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A21" s="15">
+      <c r="A21" s="13">
         <v>44420</v>
       </c>
-      <c r="B21" s="15"/>
+      <c r="B21" s="13"/>
       <c r="D21" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
       <c r="P21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R21" s="26">
+      <c r="R21" s="23">
         <v>153</v>
       </c>
-      <c r="S21" s="26">
+      <c r="S21" s="23">
         <v>20</v>
       </c>
-      <c r="T21" s="26">
+      <c r="T21" s="23">
         <v>202</v>
       </c>
       <c r="U21" s="1" t="s">
@@ -1937,32 +1951,23 @@
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A22" s="15">
+      <c r="A22" s="13">
         <v>44425</v>
       </c>
-      <c r="B22" s="15"/>
+      <c r="B22" s="13"/>
       <c r="D22" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
       <c r="P22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R22" s="26">
+      <c r="R22" s="23">
         <v>229</v>
       </c>
-      <c r="S22" s="26">
+      <c r="S22" s="23">
         <v>58</v>
       </c>
-      <c r="T22" s="26">
+      <c r="T22" s="23">
         <v>240</v>
       </c>
       <c r="U22" s="1" t="s">
@@ -1970,32 +1975,23 @@
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A23" s="15">
+      <c r="A23" s="13">
         <v>44438</v>
       </c>
-      <c r="B23" s="15"/>
+      <c r="B23" s="13"/>
       <c r="D23" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
       <c r="P23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R23" s="26">
+      <c r="R23" s="23">
         <v>74</v>
       </c>
-      <c r="S23" s="26">
+      <c r="S23" s="23">
         <v>164</v>
       </c>
-      <c r="T23" s="26">
+      <c r="T23" s="23">
         <v>351</v>
       </c>
       <c r="U23" s="1" t="s">
@@ -2003,34 +1999,25 @@
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A24" s="15">
+      <c r="A24" s="13">
         <v>44444</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
       <c r="P24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R24" s="26">
+      <c r="R24" s="23">
         <v>305.7</v>
       </c>
-      <c r="S24" s="26">
+      <c r="S24" s="23">
         <v>350.2</v>
       </c>
-      <c r="T24" s="26">
+      <c r="T24" s="23">
         <v>177.9</v>
       </c>
       <c r="U24" s="1" t="s">
@@ -2038,32 +2025,23 @@
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A25" s="15">
+      <c r="A25" s="13">
         <v>44445</v>
       </c>
-      <c r="B25" s="15"/>
+      <c r="B25" s="13"/>
       <c r="D25" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
       <c r="P25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R25" s="26">
+      <c r="R25" s="23">
         <v>123</v>
       </c>
-      <c r="S25" s="26">
+      <c r="S25" s="23">
         <v>160</v>
       </c>
-      <c r="T25" s="26">
+      <c r="T25" s="23">
         <v>348</v>
       </c>
       <c r="U25" s="1" t="s">
@@ -2071,10 +2049,10 @@
       </c>
     </row>
     <row r="26" spans="1:27" ht="58" x14ac:dyDescent="0.35">
-      <c r="A26" s="15">
+      <c r="A26" s="13">
         <v>44449</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -2086,45 +2064,40 @@
       <c r="E26" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H26" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
+      <c r="H26" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="N26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O26" s="20" t="s">
+      <c r="O26" s="17" t="s">
         <v>47</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R26" s="26">
+      <c r="R26" s="23">
         <v>19</v>
       </c>
-      <c r="S26" s="26">
+      <c r="S26" s="23">
         <v>25.4</v>
       </c>
-      <c r="T26" s="26">
+      <c r="T26" s="23">
         <v>214.5</v>
       </c>
       <c r="U26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V26" s="21" t="s">
+      <c r="V26" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="W26" s="21"/>
+      <c r="W26" s="18"/>
       <c r="X26" s="6">
         <v>44541</v>
       </c>
@@ -2139,48 +2112,39 @@
       </c>
     </row>
     <row r="27" spans="1:27" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="15">
+      <c r="A27" s="13">
         <v>44452</v>
       </c>
-      <c r="B27" s="15"/>
+      <c r="B27" s="13"/>
       <c r="D27" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="O27" s="13"/>
+      <c r="O27" s="11"/>
       <c r="P27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R27" s="26">
+      <c r="R27" s="23">
         <v>150.4</v>
       </c>
-      <c r="S27" s="29">
+      <c r="S27" s="26">
         <v>133.69999999999999</v>
       </c>
-      <c r="T27" s="26">
+      <c r="T27" s="23">
         <v>323.60000000000002</v>
       </c>
       <c r="U27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="V27" s="12" t="s">
+      <c r="V27" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="W27" s="12"/>
+      <c r="W27" s="10"/>
     </row>
     <row r="28" spans="1:27" ht="58" x14ac:dyDescent="0.35">
-      <c r="A28" s="15">
+      <c r="A28" s="13">
         <v>44454</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -2192,20 +2156,20 @@
       <c r="E28" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H28" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
+      <c r="H28" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
       <c r="N28" s="1" t="s">
         <v>3</v>
       </c>
@@ -2215,13 +2179,13 @@
       <c r="P28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R28" s="26">
+      <c r="R28" s="23">
         <v>73.2</v>
       </c>
-      <c r="S28" s="26">
+      <c r="S28" s="23">
         <v>41.5</v>
       </c>
-      <c r="T28" s="26">
+      <c r="T28" s="23">
         <v>231.9</v>
       </c>
       <c r="U28" s="1" t="s">
@@ -2241,34 +2205,34 @@
       </c>
     </row>
     <row r="29" spans="1:27" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="15">
+      <c r="A29" s="13">
         <v>44458</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
       <c r="P29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R29" s="26">
+      <c r="R29" s="23">
         <v>33.700000000000003</v>
       </c>
-      <c r="S29" s="26">
+      <c r="S29" s="23">
         <v>331.1</v>
       </c>
-      <c r="T29" s="26">
+      <c r="T29" s="23">
         <v>162.5</v>
       </c>
       <c r="U29" s="1" t="s">
@@ -2279,22 +2243,22 @@
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A30" s="15">
+      <c r="A30" s="13">
         <v>44459</v>
       </c>
-      <c r="B30" s="15"/>
+      <c r="B30" s="13"/>
       <c r="D30" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
       <c r="P30" s="1" t="s">
         <v>36</v>
       </c>
@@ -2303,32 +2267,32 @@
       </c>
     </row>
     <row r="31" spans="1:27" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="15">
+      <c r="A31" s="13">
         <v>44462</v>
       </c>
-      <c r="B31" s="15"/>
+      <c r="B31" s="13"/>
       <c r="D31" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
       <c r="P31" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R31" s="26">
+      <c r="R31" s="23">
         <v>284.39999999999998</v>
       </c>
-      <c r="S31" s="29">
+      <c r="S31" s="26">
         <v>191.5</v>
       </c>
-      <c r="T31" s="29">
+      <c r="T31" s="26">
         <v>24</v>
       </c>
       <c r="U31" s="1" t="s">
@@ -2339,22 +2303,22 @@
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A32" s="15">
+      <c r="A32" s="13">
         <v>44465</v>
       </c>
-      <c r="B32" s="15"/>
+      <c r="B32" s="13"/>
       <c r="D32" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
       <c r="P32" s="1" t="s">
         <v>36</v>
       </c>
@@ -2363,10 +2327,10 @@
       </c>
     </row>
     <row r="33" spans="1:27" ht="87" x14ac:dyDescent="0.35">
-      <c r="A33" s="15">
+      <c r="A33" s="13">
         <v>44466</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -2378,20 +2342,15 @@
       <c r="E33" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F33" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H33" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
+      <c r="H33" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="N33" s="1" t="s">
         <v>3</v>
       </c>
@@ -2401,13 +2360,13 @@
       <c r="P33" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R33" s="26">
+      <c r="R33" s="23">
         <v>145.80000000000001</v>
       </c>
-      <c r="S33" s="26">
+      <c r="S33" s="23">
         <v>22.8</v>
       </c>
-      <c r="T33" s="26">
+      <c r="T33" s="23">
         <v>216.4</v>
       </c>
       <c r="U33" s="1" t="s">
@@ -2430,10 +2389,10 @@
       </c>
     </row>
     <row r="34" spans="1:27" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="15">
+      <c r="A34" s="13">
         <v>44486</v>
       </c>
-      <c r="B34" s="15"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="3" t="s">
         <v>49</v>
       </c>
@@ -2443,20 +2402,15 @@
       <c r="E34" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F34" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H34" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
+      <c r="H34" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="N34" s="1" t="s">
         <v>3</v>
       </c>
@@ -2466,7 +2420,7 @@
       <c r="P34" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S34" s="26">
+      <c r="S34" s="23">
         <v>179</v>
       </c>
       <c r="U34" s="1" t="s">
@@ -2489,10 +2443,10 @@
       </c>
     </row>
     <row r="35" spans="1:27" ht="58" x14ac:dyDescent="0.35">
-      <c r="A35" s="15">
+      <c r="A35" s="13">
         <v>44488</v>
       </c>
-      <c r="B35" s="15"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="3" t="s">
         <v>48</v>
       </c>
@@ -2502,20 +2456,15 @@
       <c r="E35" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H35" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
+      <c r="H35" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="N35" s="1" t="s">
         <v>3</v>
       </c>
@@ -2525,7 +2474,7 @@
       <c r="P35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S35" s="29">
+      <c r="S35" s="26">
         <v>119</v>
       </c>
       <c r="U35" s="1" t="s">
@@ -2545,10 +2494,10 @@
       </c>
     </row>
     <row r="36" spans="1:27" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="15">
+      <c r="A36" s="13">
         <v>44491</v>
       </c>
-      <c r="B36" s="15"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="3" t="s">
         <v>42</v>
       </c>
@@ -2558,20 +2507,15 @@
       <c r="E36" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F36" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H36" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
+      <c r="H36" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="N36" s="1" t="s">
         <v>3</v>
       </c>
@@ -2581,7 +2525,7 @@
       <c r="P36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S36" s="26">
+      <c r="S36" s="23">
         <v>180</v>
       </c>
       <c r="U36" s="1" t="s">
@@ -2604,22 +2548,13 @@
       </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A37" s="15">
+      <c r="A37" s="13">
         <v>44522</v>
       </c>
-      <c r="B37" s="15"/>
+      <c r="B37" s="13"/>
       <c r="D37" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
       <c r="P37" s="1" t="s">
         <v>37</v>
       </c>
@@ -2631,10 +2566,10 @@
       </c>
     </row>
     <row r="38" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="15">
+      <c r="A38" s="13">
         <v>44523</v>
       </c>
-      <c r="B38" s="15"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="3" t="s">
         <v>25</v>
       </c>
@@ -2644,20 +2579,15 @@
       <c r="E38" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H38" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
+      <c r="H38" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="N38" s="1" t="s">
         <v>3</v>
       </c>
@@ -2690,10 +2620,10 @@
       </c>
     </row>
     <row r="39" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="15">
+      <c r="A39" s="13">
         <v>44530</v>
       </c>
-      <c r="B39" s="15"/>
+      <c r="B39" s="13"/>
       <c r="C39" s="3" t="s">
         <v>31</v>
       </c>
@@ -2703,20 +2633,15 @@
       <c r="E39" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F39" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H39" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
+      <c r="H39" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="N39" s="1" t="s">
         <v>3</v>
       </c>
@@ -2729,13 +2654,13 @@
       <c r="Q39" s="1">
         <v>203</v>
       </c>
-      <c r="R39" s="26">
+      <c r="R39" s="23">
         <v>95</v>
       </c>
-      <c r="S39" s="26">
+      <c r="S39" s="23">
         <v>204</v>
       </c>
-      <c r="T39" s="26">
+      <c r="T39" s="23">
         <v>55</v>
       </c>
       <c r="U39" s="1" t="s">
@@ -2758,10 +2683,10 @@
       </c>
     </row>
     <row r="40" spans="1:27" ht="87" x14ac:dyDescent="0.35">
-      <c r="A40" s="15">
+      <c r="A40" s="13">
         <v>44532</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -2773,20 +2698,15 @@
       <c r="E40" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="F40" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H40" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
+      <c r="H40" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="N40" s="1" t="s">
         <v>3</v>
       </c>
@@ -2799,13 +2719,13 @@
       <c r="Q40" s="1">
         <v>114</v>
       </c>
-      <c r="R40" s="26">
+      <c r="R40" s="23">
         <v>20.6</v>
       </c>
-      <c r="S40" s="29">
+      <c r="S40" s="26">
         <v>114.9</v>
       </c>
-      <c r="T40" s="26">
+      <c r="T40" s="23">
         <v>326</v>
       </c>
       <c r="U40" s="1" t="s">
@@ -2828,10 +2748,10 @@
       </c>
     </row>
     <row r="41" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="15">
+      <c r="A41" s="13">
         <v>44533</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2843,20 +2763,15 @@
       <c r="E41" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="F41" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H41" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
+      <c r="H41" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="N41" s="1" t="s">
         <v>3</v>
       </c>
@@ -2869,13 +2784,13 @@
       <c r="Q41" s="1">
         <v>265</v>
       </c>
-      <c r="R41" s="26">
+      <c r="R41" s="23">
         <v>179.2</v>
       </c>
-      <c r="S41" s="26">
+      <c r="S41" s="23">
         <v>265.8</v>
       </c>
-      <c r="T41" s="26">
+      <c r="T41" s="23">
         <v>117.2</v>
       </c>
       <c r="U41" s="1" t="s">
@@ -2898,172 +2813,172 @@
       </c>
     </row>
     <row r="42" spans="1:27" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="15">
+      <c r="A42" s="13">
         <v>44783</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E42" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F42" s="11" t="s">
+      <c r="E42" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H42" s="11" t="s">
+      <c r="H42" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J42" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K42" s="11" t="s">
+      <c r="J42" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K42" s="3" t="s">
         <v>89</v>
       </c>
       <c r="P42" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R42" s="34">
+      <c r="R42" s="29">
         <v>11.8</v>
       </c>
-      <c r="S42" s="32">
+      <c r="S42" s="28">
         <v>347.8</v>
       </c>
-      <c r="T42" s="26">
+      <c r="T42" s="23">
         <v>265.8</v>
       </c>
       <c r="U42" s="1" t="s">
         <v>4</v>
       </c>
       <c r="V42" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A43" s="15">
+      <c r="A43" s="13">
         <v>44785</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E43" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F43" s="11" t="s">
+      <c r="E43" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H43" s="11" t="s">
+      <c r="H43" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I43" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J43" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K43" s="11" t="s">
+      <c r="J43" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K43" s="3" t="s">
         <v>89</v>
       </c>
       <c r="P43" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R43" s="26">
+      <c r="R43" s="23">
         <v>335.4</v>
       </c>
-      <c r="S43" s="38">
+      <c r="S43" s="31">
         <v>296.10000000000002</v>
       </c>
-      <c r="T43" s="26">
+      <c r="T43" s="23">
         <v>214.6</v>
       </c>
       <c r="U43" s="1" t="s">
         <v>3</v>
       </c>
       <c r="V43" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A44" s="15">
+      <c r="A44" s="13">
         <v>44791</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E44" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F44" s="11" t="s">
+      <c r="E44" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H44" s="11" t="s">
+      <c r="H44" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J44" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K44" s="11" t="s">
+      <c r="J44" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K44" s="3" t="s">
         <v>89</v>
       </c>
       <c r="P44" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R44" s="26">
+      <c r="R44" s="23">
         <v>98.5</v>
       </c>
-      <c r="S44" s="32">
+      <c r="S44" s="28">
         <v>14.3</v>
       </c>
-      <c r="T44" s="26">
+      <c r="T44" s="23">
         <v>294.39999999999998</v>
       </c>
       <c r="U44" s="1" t="s">
         <v>4</v>
       </c>
       <c r="V44" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="15">
+      <c r="A45" s="13">
         <v>44801</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E45" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F45" s="11" t="s">
+      <c r="E45" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H45" s="11" t="s">
+      <c r="H45" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I45" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="J45" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K45" s="11" t="s">
+      <c r="J45" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K45" s="3" t="s">
         <v>89</v>
       </c>
       <c r="L45" s="3" t="s">
@@ -3072,48 +2987,48 @@
       <c r="P45" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R45" s="26">
+      <c r="R45" s="23">
         <v>186.7</v>
       </c>
-      <c r="S45" s="32">
+      <c r="S45" s="28">
         <v>26.7</v>
       </c>
-      <c r="T45" s="26">
+      <c r="T45" s="23">
         <v>309.39999999999998</v>
       </c>
       <c r="U45" s="1" t="s">
         <v>4</v>
       </c>
       <c r="V45" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="15">
+      <c r="A46" s="13">
         <v>44803</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E46" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F46" s="11" t="s">
+      <c r="E46" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H46" s="11" t="s">
+      <c r="H46" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I46" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="J46" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K46" s="11" t="s">
+      <c r="J46" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K46" s="3" t="s">
         <v>89</v>
       </c>
       <c r="L46" s="3" t="s">
@@ -3122,13 +3037,13 @@
       <c r="P46" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R46" s="26">
+      <c r="R46" s="23">
         <v>137.19999999999999</v>
       </c>
-      <c r="S46" s="38">
+      <c r="S46" s="35">
         <v>322</v>
       </c>
-      <c r="T46" s="26">
+      <c r="T46" s="23">
         <v>245.2</v>
       </c>
       <c r="U46" s="1" t="s">
@@ -3136,31 +3051,31 @@
       </c>
     </row>
     <row r="47" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="15">
+      <c r="A47" s="13">
         <v>44805</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E47" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F47" s="11" t="s">
+      <c r="E47" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H47" s="11" t="s">
+      <c r="H47" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="J47" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K47" s="11" t="s">
+      <c r="J47" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K47" s="3" t="s">
         <v>89</v>
       </c>
       <c r="L47" s="3" t="s">
@@ -3169,48 +3084,48 @@
       <c r="P47" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R47" s="26">
+      <c r="R47" s="23">
         <v>96.8</v>
       </c>
-      <c r="S47" s="38">
+      <c r="S47" s="31">
         <v>266.3</v>
       </c>
-      <c r="T47" s="26">
+      <c r="T47" s="23">
         <v>190.1</v>
       </c>
       <c r="U47" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="V47" s="2" t="s">
-        <v>117</v>
+      <c r="V47" s="7" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="15">
+      <c r="A48" s="13">
         <v>44808</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E48" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F48" s="11" t="s">
+      <c r="E48" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H48" s="11" t="s">
+      <c r="H48" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I48" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="J48" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K48" s="11" t="s">
+      <c r="J48" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K48" s="3" t="s">
         <v>89</v>
       </c>
       <c r="L48" s="3" t="s">
@@ -3219,13 +3134,13 @@
       <c r="P48" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R48" s="36">
+      <c r="R48" s="30">
         <v>231.2</v>
       </c>
-      <c r="S48" s="32">
+      <c r="S48" s="28">
         <v>17.600000000000001</v>
       </c>
-      <c r="T48" s="26">
+      <c r="T48" s="23">
         <v>302.2</v>
       </c>
       <c r="U48" s="1" t="s">
@@ -3233,31 +3148,31 @@
       </c>
     </row>
     <row r="49" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="15">
+      <c r="A49" s="13">
         <v>44809</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E49" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F49" s="11" t="s">
+      <c r="E49" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H49" s="11" t="s">
+      <c r="H49" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I49" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="J49" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K49" s="11" t="s">
+      <c r="J49" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K49" s="3" t="s">
         <v>89</v>
       </c>
       <c r="L49" s="3" t="s">
@@ -3266,317 +3181,312 @@
       <c r="P49" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R49" s="34">
+      <c r="R49" s="29">
         <v>5.4</v>
       </c>
-      <c r="S49" s="39">
+      <c r="S49" s="32">
         <v>144.4</v>
       </c>
-      <c r="T49" s="26">
+      <c r="T49" s="23">
         <v>69.2</v>
       </c>
       <c r="U49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="V49" s="41" t="s">
-        <v>124</v>
+      <c r="V49" s="33" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A50" s="15">
+      <c r="A50" s="13">
         <v>44816</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E50" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F50" s="11" t="s">
+      <c r="E50" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H50" s="11" t="s">
+      <c r="H50" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I50" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J50" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K50" s="11" t="s">
+      <c r="J50" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K50" s="3" t="s">
         <v>89</v>
       </c>
       <c r="P50" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R50" s="34">
+      <c r="R50" s="29">
         <v>16</v>
       </c>
-      <c r="S50" s="26">
+      <c r="S50" s="23">
         <v>101.7</v>
       </c>
-      <c r="T50" s="26">
+      <c r="T50" s="23">
         <v>28.4</v>
       </c>
       <c r="U50" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="V50" s="41" t="s">
-        <v>124</v>
+      <c r="V50" s="33" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A51" s="15">
+      <c r="A51" s="13">
         <v>44817</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E51" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F51" s="11" t="s">
+      <c r="E51" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F51" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H51" s="11" t="s">
+      <c r="H51" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I51" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J51" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K51" s="11" t="s">
+      <c r="J51" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K51" s="3" t="s">
         <v>89</v>
       </c>
       <c r="P51" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R51" s="26">
+      <c r="R51" s="23">
         <v>152.1</v>
       </c>
-      <c r="S51" s="26">
+      <c r="S51" s="31">
         <v>230.3</v>
       </c>
-      <c r="T51" s="26">
+      <c r="T51" s="23">
         <v>157.30000000000001</v>
       </c>
       <c r="U51" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="V51" s="2" t="s">
-        <v>118</v>
+      <c r="V51" s="7" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:22" ht="29" x14ac:dyDescent="0.35">
-      <c r="A52" s="15">
+      <c r="A52" s="13">
         <v>44823</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E52" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F52" s="11" t="s">
+      <c r="E52" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F52" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H52" s="11" t="s">
+      <c r="H52" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I52" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J52" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K52" s="11" t="s">
+      <c r="J52" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K52" s="3" t="s">
         <v>89</v>
       </c>
       <c r="P52" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R52" s="34">
+      <c r="R52" s="29">
         <v>17.899999999999999</v>
       </c>
-      <c r="S52" s="32">
+      <c r="S52" s="28">
         <v>50.4</v>
       </c>
-      <c r="T52" s="26">
+      <c r="T52" s="23">
         <v>339</v>
       </c>
       <c r="U52" s="1" t="s">
         <v>4</v>
       </c>
       <c r="V52" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A53" s="15">
+      <c r="A53" s="13">
         <v>44829</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E53" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F53" s="11" t="s">
+      <c r="E53" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F53" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H53" s="11" t="s">
+      <c r="H53" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I53" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J53" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K53" s="11" t="s">
+      <c r="J53" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K53" s="3" t="s">
         <v>89</v>
       </c>
       <c r="P53" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R53" s="26">
+      <c r="R53" s="23">
         <v>296.2</v>
       </c>
-      <c r="S53" s="38">
+      <c r="S53" s="31">
         <v>282.5</v>
       </c>
-      <c r="T53" s="26">
+      <c r="T53" s="23">
         <v>212.7</v>
       </c>
       <c r="U53" s="1" t="s">
         <v>3</v>
       </c>
       <c r="V53" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A54" s="15">
+      <c r="A54" s="13">
         <v>44843</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E54" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F54" s="11" t="s">
+      <c r="E54" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H54" s="11" t="s">
+      <c r="H54" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I54" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J54" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K54" s="11" t="s">
+      <c r="J54" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K54" s="3" t="s">
         <v>89</v>
       </c>
       <c r="P54" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R54" s="26">
+      <c r="R54" s="23">
         <v>317.3</v>
       </c>
-      <c r="S54" s="31">
+      <c r="S54" s="27">
         <v>197.1</v>
       </c>
-      <c r="T54" s="26">
+      <c r="T54" s="23">
         <v>131</v>
       </c>
       <c r="U54" s="1" t="s">
         <v>3</v>
       </c>
       <c r="V54" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A55" s="15">
+      <c r="A55" s="13">
         <v>44843</v>
       </c>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="11"/>
-      <c r="R55" s="26">
+      <c r="R55" s="23">
         <v>267</v>
       </c>
-      <c r="S55" s="39">
+      <c r="S55" s="32">
         <v>147</v>
       </c>
-      <c r="T55" s="26">
+      <c r="T55" s="23">
         <v>81</v>
       </c>
       <c r="V55" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A56" s="15">
+      <c r="A56" s="13">
         <v>44847</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E56" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F56" s="11" t="s">
+      <c r="E56" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F56" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H56" s="11" t="s">
+      <c r="H56" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J56" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K56" s="11" t="s">
+      <c r="J56" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K56" s="3" t="s">
         <v>89</v>
       </c>
       <c r="P56" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R56" s="26">
+      <c r="R56" s="23">
         <v>168.9</v>
       </c>
-      <c r="S56" s="32">
+      <c r="S56" s="28">
         <v>18.7</v>
       </c>
-      <c r="T56" s="26">
+      <c r="T56" s="23">
         <v>313.60000000000002</v>
       </c>
       <c r="U56" s="1" t="s">
@@ -3584,90 +3494,90 @@
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A57" s="15">
+      <c r="A57" s="13">
         <v>44853</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E57" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F57" s="11" t="s">
+      <c r="E57" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H57" s="11" t="s">
+      <c r="H57" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I57" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J57" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K57" s="11" t="s">
+      <c r="J57" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K57" s="3" t="s">
         <v>89</v>
       </c>
       <c r="P57" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R57" s="34">
+      <c r="R57" s="29">
         <v>34.9</v>
       </c>
-      <c r="S57" s="31">
+      <c r="S57" s="27">
         <v>198.9</v>
       </c>
-      <c r="T57" s="26">
+      <c r="T57" s="23">
         <v>135.4</v>
       </c>
       <c r="U57" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="V57" s="41" t="s">
-        <v>124</v>
+      <c r="V57" s="33" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A58" s="15">
+      <c r="A58" s="13">
         <v>44854</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E58" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F58" s="11" t="s">
+      <c r="E58" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F58" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H58" s="11" t="s">
+      <c r="H58" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J58" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K58" s="11" t="s">
+      <c r="J58" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K58" s="3" t="s">
         <v>89</v>
       </c>
       <c r="P58" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R58" s="35">
+      <c r="R58" s="36">
         <v>228</v>
       </c>
-      <c r="S58" s="33">
+      <c r="S58" s="37">
         <v>24.1</v>
       </c>
-      <c r="T58" s="30">
+      <c r="T58" s="38">
         <v>320.89999999999998</v>
       </c>
       <c r="U58" s="1" t="s">
@@ -3675,78 +3585,78 @@
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A59" s="15">
+      <c r="A59" s="13">
         <v>44855</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E59" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F59" s="11" t="s">
+      <c r="E59" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F59" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H59" s="11" t="s">
+      <c r="H59" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J59" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K59" s="11" t="s">
+      <c r="J59" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K59" s="3" t="s">
         <v>89</v>
       </c>
       <c r="P59" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="R59" s="37">
+      <c r="R59" s="39">
         <v>0.3</v>
       </c>
       <c r="S59" s="40">
         <v>149</v>
       </c>
-      <c r="T59" s="30">
+      <c r="T59" s="38">
         <v>86.1</v>
       </c>
       <c r="U59" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="V59" s="42" t="s">
-        <v>124</v>
+      <c r="V59" s="34" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A60" s="15">
+      <c r="A60" s="13">
         <v>44865</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E60" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F60" s="11" t="s">
+      <c r="E60" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F60" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H60" s="11" t="s">
+      <c r="H60" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I60" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J60" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K60" s="11" t="s">
+      <c r="J60" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K60" s="3" t="s">
         <v>89</v>
       </c>
       <c r="P60" s="1" t="s">
@@ -3757,31 +3667,31 @@
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A61" s="15">
+      <c r="A61" s="13">
         <v>44866</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E61" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F61" s="11" t="s">
+      <c r="E61" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H61" s="11" t="s">
+      <c r="H61" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I61" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J61" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K61" s="11" t="s">
+      <c r="J61" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K61" s="3" t="s">
         <v>89</v>
       </c>
       <c r="P61" s="1" t="s">
@@ -3792,31 +3702,31 @@
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A62" s="15">
+      <c r="A62" s="13">
         <v>44874</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E62" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F62" s="11" t="s">
+      <c r="E62" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F62" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H62" s="11" t="s">
+      <c r="H62" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I62" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J62" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K62" s="11" t="s">
+      <c r="J62" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K62" s="3" t="s">
         <v>89</v>
       </c>
       <c r="P62" s="1" t="s">
@@ -3827,31 +3737,31 @@
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A63" s="15">
+      <c r="A63" s="13">
         <v>44886</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E63" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F63" s="11" t="s">
+      <c r="E63" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>89</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H63" s="11" t="s">
+      <c r="H63" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I63" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J63" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K63" s="11" t="s">
+      <c r="J63" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K63" s="3" t="s">
         <v>89</v>
       </c>
       <c r="P63" s="1" t="s">
@@ -3859,40 +3769,40 @@
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A64" s="15"/>
+      <c r="A64" s="13"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A65" s="15"/>
+      <c r="A65" s="13"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A66" s="15"/>
+      <c r="A66" s="13"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A67" s="15"/>
+      <c r="A67" s="13"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A68" s="15"/>
+      <c r="A68" s="13"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A69" s="15"/>
+      <c r="A69" s="13"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A70" s="15"/>
+      <c r="A70" s="13"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A71" s="15"/>
+      <c r="A71" s="13"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A72" s="15"/>
+      <c r="A72" s="13"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A73" s="15"/>
+      <c r="A73" s="13"/>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A74" s="15"/>
+      <c r="A74" s="13"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A75" s="15"/>
+      <c r="A75" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AA62" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}"/>
@@ -3926,10 +3836,10 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates for Paper and Recognition of VLT/MUSE in prior Commit
A wide range of improvements have been made to various codes, including the addition of belt/zone labels, better NH3 absorption meridional profiles, etc. In addition, the *prior* commit included the addition of VLT/MUSE data for the BAA Webinar
</commit_message>
<xml_diff>
--- a/Jupiter Session Processing and Analysis Notes.xlsx
+++ b/Jupiter Session Processing and Analysis Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE31049-BFC7-49A1-9638-06776CD96E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C15869-A21E-48A2-9858-8C94B9B5519D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="307" xr2:uid="{05635B54-1AD3-49CD-8C06-A4005DAA2CD5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="307" xr2:uid="{05635B54-1AD3-49CD-8C06-A4005DAA2CD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Summary" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Database!$A$1:$AA$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Database!$A$1:$AA$63</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1141,39 +1141,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AA75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A52" sqref="A52:XFD52"/>
+      <selection pane="bottomRight" activeCell="S57" sqref="S57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="46.54296875" style="3" customWidth="1"/>
-    <col min="4" max="6" width="7.7265625" style="3" customWidth="1"/>
-    <col min="7" max="8" width="7.6328125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="7.81640625" style="3" customWidth="1"/>
-    <col min="10" max="12" width="6.6328125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="5.453125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" style="1"/>
-    <col min="15" max="15" width="8.7265625" style="4"/>
-    <col min="16" max="17" width="8.7265625" style="1"/>
-    <col min="18" max="18" width="8.7265625" style="23"/>
-    <col min="19" max="20" width="6.54296875" style="23" customWidth="1"/>
-    <col min="21" max="21" width="5.1796875" style="1" customWidth="1"/>
-    <col min="22" max="22" width="50.26953125" style="2" customWidth="1"/>
-    <col min="23" max="23" width="30.36328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46.5703125" style="3" customWidth="1"/>
+    <col min="4" max="6" width="7.7109375" style="3" customWidth="1"/>
+    <col min="7" max="8" width="7.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" style="3" customWidth="1"/>
+    <col min="10" max="12" width="6.5703125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" style="1"/>
+    <col min="15" max="15" width="8.7109375" style="4"/>
+    <col min="16" max="17" width="8.7109375" style="1"/>
+    <col min="18" max="18" width="8.7109375" style="23"/>
+    <col min="19" max="20" width="6.5703125" style="23" customWidth="1"/>
+    <col min="21" max="21" width="5.140625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="50.28515625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="30.42578125" style="2" customWidth="1"/>
     <col min="24" max="24" width="12" style="6" customWidth="1"/>
-    <col min="25" max="26" width="5.7265625" style="5" customWidth="1"/>
-    <col min="27" max="27" width="5.7265625" style="1" customWidth="1"/>
+    <col min="25" max="26" width="5.7109375" style="5" customWidth="1"/>
+    <col min="27" max="27" width="5.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="19" customFormat="1" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>52</v>
       </c>
@@ -1256,7 +1257,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>44032</v>
       </c>
@@ -1304,7 +1305,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>44041</v>
       </c>
@@ -1352,7 +1353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>44042</v>
       </c>
@@ -1400,7 +1401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>44043</v>
       </c>
@@ -1448,7 +1449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>44076</v>
       </c>
@@ -1463,7 +1464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>44077</v>
       </c>
@@ -1478,7 +1479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>44078</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>44087</v>
       </c>
@@ -1526,7 +1527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>44088</v>
       </c>
@@ -1559,7 +1560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>44089</v>
       </c>
@@ -1571,7 +1572,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>44098</v>
       </c>
@@ -1618,7 +1619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>44099</v>
       </c>
@@ -1654,7 +1655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>44111</v>
       </c>
@@ -1666,7 +1667,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>44112</v>
       </c>
@@ -1678,7 +1679,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>44113</v>
       </c>
@@ -1690,7 +1691,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="87" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>44369</v>
       </c>
@@ -1741,7 +1742,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>44385</v>
       </c>
@@ -1803,7 +1804,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>44396</v>
       </c>
@@ -1866,7 +1867,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="58" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>44397</v>
       </c>
@@ -1926,7 +1927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>44420</v>
       </c>
@@ -1950,7 +1951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>44425</v>
       </c>
@@ -1974,7 +1975,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>44438</v>
       </c>
@@ -1998,7 +1999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>44444</v>
       </c>
@@ -2024,7 +2025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>44445</v>
       </c>
@@ -2048,7 +2049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="58" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>44449</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:27" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>44452</v>
       </c>
@@ -2140,7 +2141,7 @@
       </c>
       <c r="W27" s="10"/>
     </row>
-    <row r="28" spans="1:27" ht="58" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>44454</v>
       </c>
@@ -2204,7 +2205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="58" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>44458</v>
       </c>
@@ -2242,7 +2243,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>44459</v>
       </c>
@@ -2266,7 +2267,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:27" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>44462</v>
       </c>
@@ -2302,7 +2303,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>44465</v>
       </c>
@@ -2326,7 +2327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="87" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:27" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>44466</v>
       </c>
@@ -2388,7 +2389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>44486</v>
       </c>
@@ -2442,7 +2443,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:27" ht="58" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>44488</v>
       </c>
@@ -2493,7 +2494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:27" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:27" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>44491</v>
       </c>
@@ -2547,7 +2548,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>44522</v>
       </c>
@@ -2565,7 +2566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:27" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>44523</v>
       </c>
@@ -2619,7 +2620,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>44530</v>
       </c>
@@ -2682,7 +2683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:27" ht="87" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:27" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>44532</v>
       </c>
@@ -2747,7 +2748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <v>44533</v>
       </c>
@@ -2812,7 +2813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>44783</v>
       </c>
@@ -2859,7 +2860,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>44785</v>
       </c>
@@ -2906,7 +2907,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>44791</v>
       </c>
@@ -2953,7 +2954,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
         <v>44801</v>
       </c>
@@ -3003,7 +3004,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>44803</v>
       </c>
@@ -3050,7 +3051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>44805</v>
       </c>
@@ -3100,7 +3101,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>44808</v>
       </c>
@@ -3147,7 +3148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:22" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>44809</v>
       </c>
@@ -3197,7 +3198,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>44816</v>
       </c>
@@ -3244,7 +3245,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>44817</v>
       </c>
@@ -3291,7 +3292,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
         <v>44823</v>
       </c>
@@ -3338,7 +3339,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="13">
         <v>44829</v>
       </c>
@@ -3385,7 +3386,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>44843</v>
       </c>
@@ -3432,7 +3433,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
         <v>44843</v>
       </c>
@@ -3449,7 +3450,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>44847</v>
       </c>
@@ -3493,7 +3494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
         <v>44853</v>
       </c>
@@ -3540,7 +3541,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>44854</v>
       </c>
@@ -3584,7 +3585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
         <v>44855</v>
       </c>
@@ -3631,7 +3632,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
         <v>44865</v>
       </c>
@@ -3666,7 +3667,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
         <v>44866</v>
       </c>
@@ -3701,7 +3702,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
         <v>44874</v>
       </c>
@@ -3736,7 +3737,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
         <v>44886</v>
       </c>
@@ -3768,44 +3769,50 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="13"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="13"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA62" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}"/>
+  <autoFilter ref="A1:AA63" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}">
+    <filterColumn colId="15">
+      <filters>
+        <filter val="CMOS"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="Y2:AA126">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"M"</formula>
@@ -3833,9 +3840,9 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>68</v>
       </c>
@@ -3843,7 +3850,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -3851,7 +3858,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -3859,102 +3866,102 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>98</v>
       </c>
@@ -3973,14 +3980,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Many Changes, First Project Commit
Beginning of re-architecture to support an efficient pipeline and the AAS/EPSC presentation in October.
</commit_message>
<xml_diff>
--- a/Jupiter Session Processing and Analysis Notes.xlsx
+++ b/Jupiter Session Processing and Analysis Notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81078A1B-E7D2-4F3C-8952-A53632B815F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C004D2C4-59FE-4D8C-BA11-B758203CC985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="560" activeTab="1" xr2:uid="{05635B54-1AD3-49CD-8C06-A4005DAA2CD5}"/>
   </bookViews>
@@ -2281,22 +2281,22 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="42" t="s">
         <v>33</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="42" t="s">
         <v>131</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="42" t="s">
         <v>127</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="43">
         <v>44014</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="43">
         <v>44018</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="43">
         <v>44022</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="43">
         <v>44032</v>
       </c>
@@ -2442,197 +2442,197 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="43">
         <v>44041</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="43">
         <v>44042</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="43">
         <v>44043</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="43">
         <v>44369</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="43">
         <v>44385</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="43">
         <v>44396</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="43">
         <v>44397</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="43">
         <v>44449</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="43">
         <v>44452</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="43">
         <v>44454</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="43">
         <v>44458</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="43">
         <v>44459</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="43">
         <v>44462</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="43">
         <v>44465</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="43">
         <v>44466</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="43">
         <v>44486</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="43">
         <v>44488</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="43">
         <v>44491</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="43">
         <v>44530</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="43">
         <v>44532</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="43">
         <v>44533</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="43">
         <v>44783</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="43">
         <v>44785</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="43">
         <v>44791</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="43">
         <v>44801</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="43">
         <v>44803</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="43">
         <v>44805</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="43">
         <v>44808</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="43">
         <v>44809</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="43">
         <v>44816</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="43">
         <v>44817</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="43">
         <v>44823</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="43">
         <v>44829</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="43">
         <v>44843</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="43">
         <v>44847</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="43">
         <v>44853</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="43">
         <v>44854</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="43">
         <v>44855</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="43" t="s">
         <v>128</v>
       </c>
@@ -2672,41 +2672,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AC87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="U79" sqref="U79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="46" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="46.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" style="46" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46.54296875" style="3" customWidth="1"/>
     <col min="4" max="4" width="13" style="4" customWidth="1"/>
-    <col min="5" max="6" width="8.7109375" style="1"/>
-    <col min="7" max="9" width="7.7109375" style="3" customWidth="1"/>
-    <col min="10" max="11" width="7.5703125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" style="3" customWidth="1"/>
-    <col min="13" max="15" width="6.5703125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="5.42578125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="8.7109375" style="1"/>
-    <col min="18" max="18" width="8.7109375" style="4"/>
-    <col min="19" max="19" width="8.7109375" style="1"/>
-    <col min="20" max="20" width="8.7109375" style="23"/>
-    <col min="21" max="22" width="6.5703125" style="23" customWidth="1"/>
-    <col min="23" max="23" width="5.140625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="50.28515625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="30.42578125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="8.7265625" style="1"/>
+    <col min="7" max="9" width="7.7265625" style="3" customWidth="1"/>
+    <col min="10" max="11" width="7.54296875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="7.81640625" style="3" customWidth="1"/>
+    <col min="13" max="15" width="6.54296875" style="3" customWidth="1"/>
+    <col min="16" max="16" width="5.453125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="8.7265625" style="1"/>
+    <col min="18" max="18" width="8.7265625" style="4"/>
+    <col min="19" max="19" width="8.7265625" style="1"/>
+    <col min="20" max="20" width="8.7265625" style="23"/>
+    <col min="21" max="22" width="6.54296875" style="23" customWidth="1"/>
+    <col min="23" max="23" width="5.1796875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="50.26953125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="30.453125" style="2" customWidth="1"/>
     <col min="26" max="26" width="12" style="6" customWidth="1"/>
-    <col min="27" max="28" width="5.7109375" style="5" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" style="1" customWidth="1"/>
+    <col min="27" max="28" width="5.7265625" style="5" customWidth="1"/>
+    <col min="29" max="29" width="5.7265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
         <v>52</v>
       </c>
@@ -2795,7 +2798,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="45">
         <v>44014</v>
       </c>
@@ -2831,7 +2834,7 @@
       <c r="AB2" s="21"/>
       <c r="AC2" s="20"/>
     </row>
-    <row r="3" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="45">
         <v>44014</v>
       </c>
@@ -2867,7 +2870,7 @@
       <c r="AB3" s="21"/>
       <c r="AC3" s="20"/>
     </row>
-    <row r="4" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="45">
         <v>44014</v>
       </c>
@@ -2903,7 +2906,7 @@
       <c r="AB4" s="21"/>
       <c r="AC4" s="20"/>
     </row>
-    <row r="5" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="45">
         <v>44014</v>
       </c>
@@ -2939,7 +2942,7 @@
       <c r="AB5" s="21"/>
       <c r="AC5" s="20"/>
     </row>
-    <row r="6" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="45">
         <v>44018</v>
       </c>
@@ -2975,7 +2978,7 @@
       <c r="AB6" s="21"/>
       <c r="AC6" s="20"/>
     </row>
-    <row r="7" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="45">
         <v>44018</v>
       </c>
@@ -3011,7 +3014,7 @@
       <c r="AB7" s="21"/>
       <c r="AC7" s="20"/>
     </row>
-    <row r="8" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="45">
         <v>44018</v>
       </c>
@@ -3047,7 +3050,7 @@
       <c r="AB8" s="21"/>
       <c r="AC8" s="20"/>
     </row>
-    <row r="9" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="45">
         <v>44018</v>
       </c>
@@ -3083,7 +3086,7 @@
       <c r="AB9" s="21"/>
       <c r="AC9" s="20"/>
     </row>
-    <row r="10" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="45">
         <v>44018</v>
       </c>
@@ -3119,7 +3122,7 @@
       <c r="AB10" s="21"/>
       <c r="AC10" s="20"/>
     </row>
-    <row r="11" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="45">
         <v>44018</v>
       </c>
@@ -3155,7 +3158,7 @@
       <c r="AB11" s="21"/>
       <c r="AC11" s="20"/>
     </row>
-    <row r="12" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="45">
         <v>44018</v>
       </c>
@@ -3191,7 +3194,7 @@
       <c r="AB12" s="21"/>
       <c r="AC12" s="20"/>
     </row>
-    <row r="13" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="45">
         <v>44022</v>
       </c>
@@ -3227,7 +3230,7 @@
       <c r="AB13" s="21"/>
       <c r="AC13" s="20"/>
     </row>
-    <row r="14" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="45">
         <v>44022</v>
       </c>
@@ -3263,7 +3266,7 @@
       <c r="AB14" s="21"/>
       <c r="AC14" s="20"/>
     </row>
-    <row r="15" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="45">
         <v>44022</v>
       </c>
@@ -3299,7 +3302,7 @@
       <c r="AB15" s="21"/>
       <c r="AC15" s="20"/>
     </row>
-    <row r="16" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="45">
         <v>44022</v>
       </c>
@@ -3335,7 +3338,7 @@
       <c r="AB16" s="21"/>
       <c r="AC16" s="20"/>
     </row>
-    <row r="17" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="45">
         <v>44022</v>
       </c>
@@ -3371,7 +3374,7 @@
       <c r="AB17" s="21"/>
       <c r="AC17" s="20"/>
     </row>
-    <row r="18" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="45">
         <v>44022</v>
       </c>
@@ -3407,7 +3410,7 @@
       <c r="AB18" s="21"/>
       <c r="AC18" s="20"/>
     </row>
-    <row r="19" spans="1:29" s="19" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="45">
         <v>44022</v>
       </c>
@@ -3443,7 +3446,7 @@
       <c r="AB19" s="21"/>
       <c r="AC19" s="20"/>
     </row>
-    <row r="20" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="46">
         <v>44032</v>
       </c>
@@ -3497,7 +3500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A21" s="46">
         <v>44032</v>
       </c>
@@ -3509,7 +3512,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A22" s="46">
         <v>44032</v>
       </c>
@@ -3521,7 +3524,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A23" s="46">
         <v>44032</v>
       </c>
@@ -3533,7 +3536,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A24" s="46">
         <v>44032</v>
       </c>
@@ -3545,7 +3548,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A25" s="46">
         <v>44032</v>
       </c>
@@ -3557,7 +3560,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A26" s="46">
         <v>44032</v>
       </c>
@@ -3569,7 +3572,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:29" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A27" s="46">
         <v>44041</v>
       </c>
@@ -3617,7 +3620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" s="46">
         <v>44042</v>
       </c>
@@ -3665,7 +3668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:29" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="46">
         <v>44043</v>
       </c>
@@ -3713,7 +3716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A30" s="46">
         <v>44076</v>
       </c>
@@ -3728,7 +3731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A31" s="46">
         <v>44077</v>
       </c>
@@ -3743,7 +3746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A32" s="46">
         <v>44078</v>
       </c>
@@ -3758,7 +3761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="46">
         <v>44087</v>
       </c>
@@ -3791,7 +3794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:29" ht="150" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A34" s="46">
         <v>44088</v>
       </c>
@@ -3824,7 +3827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A35" s="46">
         <v>44089</v>
       </c>
@@ -3836,7 +3839,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="46">
         <v>44098</v>
       </c>
@@ -3883,7 +3886,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:29" ht="105" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A37" s="46">
         <v>44099</v>
       </c>
@@ -3919,7 +3922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A38" s="46">
         <v>44111</v>
       </c>
@@ -3931,7 +3934,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A39" s="46">
         <v>44112</v>
       </c>
@@ -3943,7 +3946,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A40" s="46">
         <v>44113</v>
       </c>
@@ -3955,7 +3958,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:29" ht="105" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" ht="87" x14ac:dyDescent="0.35">
       <c r="A41" s="46">
         <v>44369</v>
       </c>
@@ -4006,7 +4009,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:29" ht="90" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A42" s="46">
         <v>44385</v>
       </c>
@@ -4069,7 +4072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:29" ht="120" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A43" s="46">
         <v>44396</v>
       </c>
@@ -4133,7 +4136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:29" ht="58" x14ac:dyDescent="0.35">
       <c r="A44" s="46">
         <v>44397</v>
       </c>
@@ -4193,7 +4196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A45" s="46">
         <v>44420</v>
       </c>
@@ -4217,7 +4220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A46" s="46">
         <v>44425</v>
       </c>
@@ -4241,7 +4244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A47" s="46">
         <v>44438</v>
       </c>
@@ -4265,7 +4268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A48" s="46">
         <v>44444</v>
       </c>
@@ -4291,7 +4294,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A49" s="46">
         <v>44445</v>
       </c>
@@ -4315,7 +4318,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:29" ht="58" x14ac:dyDescent="0.35">
       <c r="A50" s="46">
         <v>44449</v>
       </c>
@@ -4378,7 +4381,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:29" ht="120" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A51" s="46">
         <v>44452</v>
       </c>
@@ -4407,7 +4410,7 @@
       </c>
       <c r="Y51" s="10"/>
     </row>
-    <row r="52" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:29" ht="58" x14ac:dyDescent="0.35">
       <c r="A52" s="46">
         <v>44454</v>
       </c>
@@ -4471,7 +4474,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:29" ht="58" x14ac:dyDescent="0.35">
       <c r="A53" s="46">
         <v>44458</v>
       </c>
@@ -4509,7 +4512,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A54" s="46">
         <v>44459</v>
       </c>
@@ -4533,7 +4536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:29" ht="120" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:29" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A55" s="46">
         <v>44462</v>
       </c>
@@ -4569,7 +4572,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A56" s="46">
         <v>44465</v>
       </c>
@@ -4593,7 +4596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:29" ht="90" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:29" ht="87" x14ac:dyDescent="0.35">
       <c r="A57" s="46">
         <v>44466</v>
       </c>
@@ -4655,7 +4658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:29" ht="75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:29" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A58" s="46">
         <v>44486</v>
       </c>
@@ -4709,7 +4712,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:29" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:29" ht="58" x14ac:dyDescent="0.35">
       <c r="A59" s="46">
         <v>44488</v>
       </c>
@@ -4760,7 +4763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:29" ht="105" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:29" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A60" s="46">
         <v>44491</v>
       </c>
@@ -4814,7 +4817,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A61" s="46">
         <v>44522</v>
       </c>
@@ -4832,7 +4835,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A62" s="46">
         <v>44523</v>
       </c>
@@ -4886,7 +4889,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A63" s="46">
         <v>44530</v>
       </c>
@@ -4949,7 +4952,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:29" ht="90" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:29" ht="87" x14ac:dyDescent="0.35">
       <c r="A64" s="46">
         <v>44532</v>
       </c>
@@ -5014,7 +5017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A65" s="46">
         <v>44533</v>
       </c>
@@ -5079,7 +5082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:29" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="46">
         <v>44783</v>
       </c>
@@ -5126,7 +5129,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A67" s="46">
         <v>44785</v>
       </c>
@@ -5173,7 +5176,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A68" s="46">
         <v>44791</v>
       </c>
@@ -5220,7 +5223,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="69" spans="1:29" ht="75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A69" s="46">
         <v>44801</v>
       </c>
@@ -5270,7 +5273,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="1:29" ht="75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A70" s="46">
         <v>44803</v>
       </c>
@@ -5317,7 +5320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:29" ht="75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A71" s="46">
         <v>44805</v>
       </c>
@@ -5367,7 +5370,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="72" spans="1:29" ht="75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A72" s="46">
         <v>44808</v>
       </c>
@@ -5414,7 +5417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:29" ht="75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A73" s="46">
         <v>44809</v>
       </c>
@@ -5464,7 +5467,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A74" s="46">
         <v>44816</v>
       </c>
@@ -5511,7 +5514,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A75" s="46">
         <v>44817</v>
       </c>
@@ -5558,7 +5561,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="76" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:29" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="46">
         <v>44823</v>
       </c>
@@ -5605,7 +5608,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A77" s="46">
         <v>44829</v>
       </c>
@@ -5652,7 +5655,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A78" s="46">
         <v>44843</v>
       </c>
@@ -5699,7 +5702,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A79" s="46">
         <v>44843</v>
       </c>
@@ -5716,7 +5719,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A80" s="46">
         <v>44847</v>
       </c>
@@ -5760,7 +5763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A81" s="46">
         <v>44853</v>
       </c>
@@ -5807,7 +5810,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A82" s="46">
         <v>44854</v>
       </c>
@@ -5851,7 +5854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A83" s="46">
         <v>44855</v>
       </c>
@@ -5898,7 +5901,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A84" s="46">
         <v>44865</v>
       </c>
@@ -5933,7 +5936,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A85" s="46">
         <v>44866</v>
       </c>
@@ -5968,7 +5971,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A86" s="46">
         <v>44874</v>
       </c>
@@ -6003,7 +6006,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A87" s="46">
         <v>44886</v>
       </c>
@@ -6051,8 +6054,9 @@
   <hyperlinks>
     <hyperlink ref="Y43" r:id="rId1" xr:uid="{3D2860D4-0BB9-43F2-9E0D-7FF2D1C83DD1}"/>
   </hyperlinks>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup scale="36" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -6082,9 +6086,9 @@
       <selection activeCell="B3" sqref="B2:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>68</v>
       </c>
@@ -6092,7 +6096,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -6100,7 +6104,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -6108,102 +6112,102 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
Pre-trip commit - Lots of updated data
Really ran through 2022 and much of 2023 to produce FITS files etc.
</commit_message>
<xml_diff>
--- a/Jupiter Session Processing and Analysis Notes.xlsx
+++ b/Jupiter Session Processing and Analysis Notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C004D2C4-59FE-4D8C-BA11-B758203CC985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5725A77B-0BBD-4599-B375-F8A8B7D8EFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="560" activeTab="1" xr2:uid="{05635B54-1AD3-49CD-8C06-A4005DAA2CD5}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="133">
   <si>
     <t>2020-07-20-0457_9-Jupiter-NoWV-NH3Abs656-0.9to1.1scale_MapFlattened-CM2_L360_MAP-BARE.png</t>
   </si>
@@ -559,6 +559,9 @@
   </si>
   <si>
     <t>Sum of Exp</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -623,7 +626,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -678,6 +681,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -692,7 +719,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -823,9 +850,27 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2675,18 +2720,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC87"/>
+  <dimension ref="A1:AC118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E96" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U79" sqref="U79"/>
+      <selection pane="bottomRight" activeCell="U104" sqref="U104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" style="46" customWidth="1"/>
+    <col min="1" max="1" width="11.7265625" style="45" customWidth="1"/>
     <col min="2" max="2" width="10.453125" style="1" customWidth="1"/>
     <col min="3" max="3" width="46.54296875" style="3" customWidth="1"/>
     <col min="4" max="4" width="13" style="4" customWidth="1"/>
@@ -2799,7 +2844,7 @@
       </c>
     </row>
     <row r="2" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="45">
+      <c r="A2" s="49">
         <v>44014</v>
       </c>
       <c r="B2" s="20"/>
@@ -2835,7 +2880,7 @@
       <c r="AC2" s="20"/>
     </row>
     <row r="3" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="45">
+      <c r="A3" s="49">
         <v>44014</v>
       </c>
       <c r="B3" s="20"/>
@@ -2871,7 +2916,7 @@
       <c r="AC3" s="20"/>
     </row>
     <row r="4" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="45">
+      <c r="A4" s="49">
         <v>44014</v>
       </c>
       <c r="B4" s="20"/>
@@ -2907,7 +2952,7 @@
       <c r="AC4" s="20"/>
     </row>
     <row r="5" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="45">
+      <c r="A5" s="49">
         <v>44014</v>
       </c>
       <c r="B5" s="20"/>
@@ -2943,7 +2988,7 @@
       <c r="AC5" s="20"/>
     </row>
     <row r="6" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="45">
+      <c r="A6" s="49">
         <v>44018</v>
       </c>
       <c r="B6" s="20"/>
@@ -2979,7 +3024,7 @@
       <c r="AC6" s="20"/>
     </row>
     <row r="7" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="45">
+      <c r="A7" s="49">
         <v>44018</v>
       </c>
       <c r="B7" s="20"/>
@@ -3015,7 +3060,7 @@
       <c r="AC7" s="20"/>
     </row>
     <row r="8" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="45">
+      <c r="A8" s="49">
         <v>44018</v>
       </c>
       <c r="B8" s="20"/>
@@ -3051,7 +3096,7 @@
       <c r="AC8" s="20"/>
     </row>
     <row r="9" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="45">
+      <c r="A9" s="49">
         <v>44018</v>
       </c>
       <c r="B9" s="20"/>
@@ -3087,7 +3132,7 @@
       <c r="AC9" s="20"/>
     </row>
     <row r="10" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="45">
+      <c r="A10" s="49">
         <v>44018</v>
       </c>
       <c r="B10" s="20"/>
@@ -3123,7 +3168,7 @@
       <c r="AC10" s="20"/>
     </row>
     <row r="11" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="45">
+      <c r="A11" s="49">
         <v>44018</v>
       </c>
       <c r="B11" s="20"/>
@@ -3159,7 +3204,7 @@
       <c r="AC11" s="20"/>
     </row>
     <row r="12" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="45">
+      <c r="A12" s="49">
         <v>44018</v>
       </c>
       <c r="B12" s="20"/>
@@ -3195,7 +3240,7 @@
       <c r="AC12" s="20"/>
     </row>
     <row r="13" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="45">
+      <c r="A13" s="49">
         <v>44022</v>
       </c>
       <c r="B13" s="20"/>
@@ -3231,7 +3276,7 @@
       <c r="AC13" s="20"/>
     </row>
     <row r="14" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="45">
+      <c r="A14" s="49">
         <v>44022</v>
       </c>
       <c r="B14" s="20"/>
@@ -3267,7 +3312,7 @@
       <c r="AC14" s="20"/>
     </row>
     <row r="15" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="45">
+      <c r="A15" s="49">
         <v>44022</v>
       </c>
       <c r="B15" s="20"/>
@@ -3303,7 +3348,7 @@
       <c r="AC15" s="20"/>
     </row>
     <row r="16" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="45">
+      <c r="A16" s="49">
         <v>44022</v>
       </c>
       <c r="B16" s="20"/>
@@ -3339,7 +3384,7 @@
       <c r="AC16" s="20"/>
     </row>
     <row r="17" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="45">
+      <c r="A17" s="49">
         <v>44022</v>
       </c>
       <c r="B17" s="20"/>
@@ -3375,7 +3420,7 @@
       <c r="AC17" s="20"/>
     </row>
     <row r="18" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="45">
+      <c r="A18" s="49">
         <v>44022</v>
       </c>
       <c r="B18" s="20"/>
@@ -3411,7 +3456,7 @@
       <c r="AC18" s="20"/>
     </row>
     <row r="19" spans="1:29" s="19" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="45">
+      <c r="A19" s="49">
         <v>44022</v>
       </c>
       <c r="B19" s="20"/>
@@ -3447,7 +3492,7 @@
       <c r="AC19" s="20"/>
     </row>
     <row r="20" spans="1:29" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="46">
+      <c r="A20" s="50">
         <v>44032</v>
       </c>
       <c r="B20" s="13"/>
@@ -3501,7 +3546,7 @@
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A21" s="46">
+      <c r="A21" s="50">
         <v>44032</v>
       </c>
       <c r="B21" s="13"/>
@@ -3513,7 +3558,7 @@
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A22" s="46">
+      <c r="A22" s="50">
         <v>44032</v>
       </c>
       <c r="B22" s="13"/>
@@ -3525,7 +3570,7 @@
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A23" s="46">
+      <c r="A23" s="50">
         <v>44032</v>
       </c>
       <c r="B23" s="13"/>
@@ -3537,7 +3582,7 @@
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A24" s="46">
+      <c r="A24" s="50">
         <v>44032</v>
       </c>
       <c r="B24" s="13"/>
@@ -3549,7 +3594,7 @@
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A25" s="46">
+      <c r="A25" s="50">
         <v>44032</v>
       </c>
       <c r="B25" s="13"/>
@@ -3561,7 +3606,7 @@
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A26" s="46">
+      <c r="A26" s="50">
         <v>44032</v>
       </c>
       <c r="B26" s="13"/>
@@ -3573,7 +3618,7 @@
       </c>
     </row>
     <row r="27" spans="1:29" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="46">
+      <c r="A27" s="50">
         <v>44041</v>
       </c>
       <c r="B27" s="13"/>
@@ -3621,7 +3666,7 @@
       </c>
     </row>
     <row r="28" spans="1:29" ht="58" x14ac:dyDescent="0.35">
-      <c r="A28" s="46">
+      <c r="A28" s="50">
         <v>44042</v>
       </c>
       <c r="B28" s="13"/>
@@ -3669,7 +3714,7 @@
       </c>
     </row>
     <row r="29" spans="1:29" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="46">
+      <c r="A29" s="50">
         <v>44043</v>
       </c>
       <c r="B29" s="13"/>
@@ -3717,7 +3762,7 @@
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A30" s="46">
+      <c r="A30" s="50">
         <v>44076</v>
       </c>
       <c r="B30" s="13"/>
@@ -3732,7 +3777,7 @@
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A31" s="46">
+      <c r="A31" s="50">
         <v>44077</v>
       </c>
       <c r="B31" s="13"/>
@@ -3747,7 +3792,7 @@
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A32" s="46">
+      <c r="A32" s="50">
         <v>44078</v>
       </c>
       <c r="B32" s="13"/>
@@ -3762,7 +3807,7 @@
       </c>
     </row>
     <row r="33" spans="1:29" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="46">
+      <c r="A33" s="50">
         <v>44087</v>
       </c>
       <c r="B33" s="13"/>
@@ -3795,7 +3840,7 @@
       </c>
     </row>
     <row r="34" spans="1:29" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="46">
+      <c r="A34" s="50">
         <v>44088</v>
       </c>
       <c r="B34" s="13"/>
@@ -3828,7 +3873,7 @@
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A35" s="46">
+      <c r="A35" s="50">
         <v>44089</v>
       </c>
       <c r="B35" s="13"/>
@@ -3840,7 +3885,7 @@
       </c>
     </row>
     <row r="36" spans="1:29" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="46">
+      <c r="A36" s="50">
         <v>44098</v>
       </c>
       <c r="B36" s="13"/>
@@ -3887,7 +3932,7 @@
       </c>
     </row>
     <row r="37" spans="1:29" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="46">
+      <c r="A37" s="50">
         <v>44099</v>
       </c>
       <c r="B37" s="13"/>
@@ -3923,7 +3968,7 @@
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A38" s="46">
+      <c r="A38" s="50">
         <v>44111</v>
       </c>
       <c r="B38" s="13"/>
@@ -3935,7 +3980,7 @@
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A39" s="46">
+      <c r="A39" s="50">
         <v>44112</v>
       </c>
       <c r="B39" s="13"/>
@@ -3947,7 +3992,7 @@
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A40" s="46">
+      <c r="A40" s="50">
         <v>44113</v>
       </c>
       <c r="B40" s="13"/>
@@ -5083,7 +5128,7 @@
       </c>
     </row>
     <row r="66" spans="1:29" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="46">
+      <c r="A66" s="47">
         <v>44783</v>
       </c>
       <c r="E66" s="1" t="s">
@@ -5130,7 +5175,7 @@
       </c>
     </row>
     <row r="67" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A67" s="46">
+      <c r="A67" s="47">
         <v>44785</v>
       </c>
       <c r="E67" s="1" t="s">
@@ -5177,7 +5222,7 @@
       </c>
     </row>
     <row r="68" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A68" s="46">
+      <c r="A68" s="47">
         <v>44791</v>
       </c>
       <c r="E68" s="1" t="s">
@@ -5224,7 +5269,7 @@
       </c>
     </row>
     <row r="69" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="46">
+      <c r="A69" s="47">
         <v>44801</v>
       </c>
       <c r="E69" s="1" t="s">
@@ -5274,7 +5319,7 @@
       </c>
     </row>
     <row r="70" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="46">
+      <c r="A70" s="47">
         <v>44803</v>
       </c>
       <c r="E70" s="1" t="s">
@@ -5321,7 +5366,7 @@
       </c>
     </row>
     <row r="71" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="46">
+      <c r="A71" s="47">
         <v>44805</v>
       </c>
       <c r="E71" s="1" t="s">
@@ -5371,7 +5416,7 @@
       </c>
     </row>
     <row r="72" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="46">
+      <c r="A72" s="47">
         <v>44808</v>
       </c>
       <c r="E72" s="1" t="s">
@@ -5418,7 +5463,7 @@
       </c>
     </row>
     <row r="73" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="46">
+      <c r="A73" s="47">
         <v>44809</v>
       </c>
       <c r="E73" s="1" t="s">
@@ -5468,7 +5513,7 @@
       </c>
     </row>
     <row r="74" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A74" s="46">
+      <c r="A74" s="47">
         <v>44816</v>
       </c>
       <c r="E74" s="1" t="s">
@@ -5515,7 +5560,7 @@
       </c>
     </row>
     <row r="75" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A75" s="46">
+      <c r="A75" s="47">
         <v>44817</v>
       </c>
       <c r="E75" s="1" t="s">
@@ -5562,7 +5607,7 @@
       </c>
     </row>
     <row r="76" spans="1:29" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="46">
+      <c r="A76" s="47">
         <v>44823</v>
       </c>
       <c r="E76" s="1" t="s">
@@ -5609,7 +5654,7 @@
       </c>
     </row>
     <row r="77" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A77" s="46">
+      <c r="A77" s="47">
         <v>44829</v>
       </c>
       <c r="E77" s="1" t="s">
@@ -5656,7 +5701,7 @@
       </c>
     </row>
     <row r="78" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A78" s="46">
+      <c r="A78" s="47">
         <v>44843</v>
       </c>
       <c r="E78" s="1" t="s">
@@ -5703,7 +5748,7 @@
       </c>
     </row>
     <row r="79" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A79" s="46">
+      <c r="A79" s="47">
         <v>44843</v>
       </c>
       <c r="T79" s="23">
@@ -5720,7 +5765,7 @@
       </c>
     </row>
     <row r="80" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A80" s="46">
+      <c r="A80" s="47">
         <v>44847</v>
       </c>
       <c r="E80" s="1" t="s">
@@ -5764,7 +5809,7 @@
       </c>
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A81" s="46">
+      <c r="A81" s="47">
         <v>44853</v>
       </c>
       <c r="E81" s="1" t="s">
@@ -5811,7 +5856,7 @@
       </c>
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A82" s="46">
+      <c r="A82" s="47">
         <v>44854</v>
       </c>
       <c r="E82" s="1" t="s">
@@ -5855,7 +5900,7 @@
       </c>
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A83" s="46">
+      <c r="A83" s="47">
         <v>44855</v>
       </c>
       <c r="E83" s="1" t="s">
@@ -5902,7 +5947,7 @@
       </c>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A84" s="46">
+      <c r="A84" s="47">
         <v>44865</v>
       </c>
       <c r="E84" s="1" t="s">
@@ -5924,20 +5969,14 @@
         <v>87</v>
       </c>
       <c r="L84" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="M84" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="N84" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="X84" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A85" s="46">
+      <c r="A85" s="47">
         <v>44866</v>
       </c>
       <c r="E85" s="1" t="s">
@@ -5959,20 +5998,14 @@
         <v>87</v>
       </c>
       <c r="L85" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="M85" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="N85" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="X85" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A86" s="46">
+      <c r="A86" s="47">
         <v>44874</v>
       </c>
       <c r="E86" s="1" t="s">
@@ -5994,20 +6027,14 @@
         <v>87</v>
       </c>
       <c r="L86" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="M86" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="N86" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="X86" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A87" s="46">
+      <c r="A87" s="47">
         <v>44886</v>
       </c>
       <c r="E87" s="1" t="s">
@@ -6029,18 +6056,1149 @@
         <v>87</v>
       </c>
       <c r="L87" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A88" s="47">
+        <v>44939</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K88" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L88" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="M87" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="N87" s="3" t="s">
-        <v>87</v>
+      <c r="M88" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N88" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U88" s="28">
+        <v>47.5</v>
+      </c>
+      <c r="W88" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A89" s="48">
+        <v>45153</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K89" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L89" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M89" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N89" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U89" s="51">
+        <v>145</v>
+      </c>
+      <c r="W89" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A90" s="48">
+        <v>45153</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L90" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M90" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N90" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U90" s="23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="91" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A91" s="48">
+        <v>45154</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I91" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K91" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L91" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M91" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N91" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U91" s="29">
+        <v>306</v>
+      </c>
+      <c r="W91" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A92" s="48">
+        <v>45155</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K92" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L92" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M92" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N92" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U92" s="52">
+        <v>91</v>
+      </c>
+      <c r="W92" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A93" s="48">
+        <v>45156</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I93" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K93" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L93" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M93" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N93" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U93" s="31">
+        <v>250</v>
+      </c>
+      <c r="W93" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A94" s="48">
+        <v>45165</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J94" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K94" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L94" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M94" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N94" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U94" s="51">
+        <v>159</v>
+      </c>
+      <c r="W94" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A95" s="48">
+        <v>45165</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I95" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J95" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K95" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L95" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M95" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N95" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U95" s="51">
+        <v>173</v>
+      </c>
+      <c r="W95" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A96" s="48">
+        <v>45168</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I96" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J96" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K96" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L96" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M96" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N96" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U96" s="31">
+        <v>258</v>
+      </c>
+      <c r="W96" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A97" s="48">
+        <v>45169</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J97" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K97" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L97" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M97" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N97" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U97" s="28">
+        <v>40</v>
+      </c>
+      <c r="W97" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A98" s="48">
+        <v>45169</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J98" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K98" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L98" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M98" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N98" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U98" s="28">
+        <v>54</v>
+      </c>
+      <c r="W98" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A99" s="48">
+        <v>45174</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H99" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I99" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J99" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K99" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L99" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M99" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N99" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U99" s="28">
+        <v>77</v>
+      </c>
+      <c r="W99" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A100" s="48">
+        <v>45174</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I100" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J100" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K100" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L100" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M100" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N100" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U100" s="52">
+        <v>93</v>
+      </c>
+      <c r="W100" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A101" s="48">
+        <v>45175</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H101" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I101" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J101" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K101" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L101" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M101" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N101" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U101" s="31">
+        <v>224</v>
+      </c>
+      <c r="W101" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A102" s="48">
+        <v>45175</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J102" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K102" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L102" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M102" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N102" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U102" s="31">
+        <v>242</v>
+      </c>
+      <c r="W102" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A103" s="48">
+        <v>45191</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H103" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I103" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J103" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K103" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L103" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M103" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N103" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U103" s="29">
+        <v>286</v>
+      </c>
+      <c r="W103" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A104" s="48">
+        <v>45193</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J104" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K104" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L104" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M104" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N104" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U104" s="28"/>
+      <c r="W104" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A105" s="48">
+        <v>45198</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H105" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I105" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J105" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K105" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L105" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M105" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N105" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W105" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A106" s="48">
+        <v>45204</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H106" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I106" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J106" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K106" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L106" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M106" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N106" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U106" s="28"/>
+      <c r="W106" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A107" s="48">
+        <v>45205</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H107" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I107" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J107" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K107" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L107" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M107" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N107" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W107" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A108" s="48">
+        <v>45205</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H108" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J108" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K108" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L108" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M108" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N108" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W108" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A109" s="48">
+        <v>45214</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H109" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I109" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J109" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K109" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L109" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M109" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N109" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U109" s="28"/>
+      <c r="W109" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A110" s="48">
+        <v>45214</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J110" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K110" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L110" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M110" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N110" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W110" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A111" s="48">
+        <v>45216</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H111" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J111" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K111" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L111" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M111" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N111" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U111" s="28"/>
+      <c r="W111" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A112" s="48">
+        <v>45216</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J112" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K112" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L112" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M112" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N112" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U112" s="28"/>
+      <c r="W112" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A113" s="48">
+        <v>45218</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H113" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I113" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J113" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K113" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L113" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M113" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N113" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U113" s="28"/>
+      <c r="W113" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A114" s="48">
+        <v>45221</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J114" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K114" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L114" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M114" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N114" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U114" s="28"/>
+      <c r="W114" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A115" s="48">
+        <v>45222</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H115" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J115" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K115" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L115" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M115" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N115" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W115" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A116" s="48">
+        <v>45222</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K116" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L116" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M116" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N116" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W116" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A117" s="48">
+        <v>45223</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H117" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J117" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K117" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L117" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M117" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N117" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W117" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A118" s="48">
+        <v>45223</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J118" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K118" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L118" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M118" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N118" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W118" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:AC87" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}"/>
-  <conditionalFormatting sqref="AA20:AC150">
+  <conditionalFormatting sqref="AA20:AC151">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"M"</formula>
     </cfRule>
@@ -6064,13 +7222,13 @@
           <x14:formula1>
             <xm:f>Validation!$B$2:$B$23</xm:f>
           </x14:formula1>
-          <xm:sqref>E1020:E1024 D2:D1024</xm:sqref>
+          <xm:sqref>E1021:E1025 D2:D1025</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{31323E06-499B-45B5-9D6B-FA064BFCB0F6}">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1019</xm:sqref>
+          <xm:sqref>E2:E1020</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Interim Update for AGU 2023
Broke out code for Mapping of L3 data from processing.
Added first trial of limb correction based on Jovian air mass factor.
Updated profile codes
</commit_message>
<xml_diff>
--- a/Jupiter Session Processing and Analysis Notes.xlsx
+++ b/Jupiter Session Processing and Analysis Notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5725A77B-0BBD-4599-B375-F8A8B7D8EFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D613F3E-29DB-429E-8949-10713C5C58DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="560" activeTab="1" xr2:uid="{05635B54-1AD3-49CD-8C06-A4005DAA2CD5}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Validation" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Database!$A$1:$AC$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Database!$A$1:$AC$122</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="133">
   <si>
     <t>2020-07-20-0457_9-Jupiter-NoWV-NH3Abs656-0.9to1.1scale_MapFlattened-CM2_L360_MAP-BARE.png</t>
   </si>
@@ -719,7 +719,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -871,6 +871,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2720,13 +2726,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC118"/>
+  <dimension ref="A1:AC122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E96" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U104" sqref="U104"/>
+      <selection pane="bottomRight" activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7196,8 +7202,148 @@
         <v>3</v>
       </c>
     </row>
+    <row r="119" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A119" s="53">
+        <v>45225</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H119" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I119" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J119" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K119" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L119" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M119" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N119" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W119" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A120" s="53">
+        <v>45233</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J120" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K120" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L120" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M120" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N120" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W120" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A121" s="54">
+        <v>45237</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H121" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J121" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K121" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L121" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M121" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N121" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W121" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A122" s="54">
+        <v>45237</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H122" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J122" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K122" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L122" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M122" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N122" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W122" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AC87" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}"/>
+  <autoFilter ref="A1:AC122" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}"/>
   <conditionalFormatting sqref="AA20:AC151">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"M"</formula>

</xml_diff>

<commit_message>
Pre-travel to AGU Release
Final changes committed before AGU
</commit_message>
<xml_diff>
--- a/Jupiter Session Processing and Analysis Notes.xlsx
+++ b/Jupiter Session Processing and Analysis Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D613F3E-29DB-429E-8949-10713C5C58DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA0BF08-6BD1-49FF-8CAB-064184E79B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="560" activeTab="1" xr2:uid="{05635B54-1AD3-49CD-8C06-A4005DAA2CD5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="560" firstSheet="1" activeTab="1" xr2:uid="{05635B54-1AD3-49CD-8C06-A4005DAA2CD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Validation" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Database!$A$1:$AC$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Database!$A$1:$AC$123</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -41,8 +41,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="133">
   <si>
     <t>2020-07-20-0457_9-Jupiter-NoWV-NH3Abs656-0.9to1.1scale_MapFlattened-CM2_L360_MAP-BARE.png</t>
   </si>
@@ -873,10 +895,10 @@
     <xf numFmtId="165" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2726,13 +2748,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC122"/>
+  <dimension ref="A1:AC173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C99" sqref="C99"/>
+      <selection pane="bottomRight" activeCell="B143" sqref="B143:B173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6701,7 +6723,9 @@
       <c r="N104" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U104" s="28"/>
+      <c r="U104" s="28">
+        <v>60</v>
+      </c>
       <c r="W104" s="1" t="s">
         <v>4</v>
       </c>
@@ -6737,6 +6761,9 @@
       <c r="N105" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="U105" s="23">
+        <v>224</v>
+      </c>
       <c r="W105" s="1" t="s">
         <v>3</v>
       </c>
@@ -6772,7 +6799,9 @@
       <c r="N106" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U106" s="28"/>
+      <c r="U106" s="28">
+        <v>27</v>
+      </c>
       <c r="W106" s="1" t="s">
         <v>4</v>
       </c>
@@ -6808,6 +6837,9 @@
       <c r="N107" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="U107" s="23">
+        <v>180</v>
+      </c>
       <c r="W107" s="1" t="s">
         <v>3</v>
       </c>
@@ -6843,6 +6875,9 @@
       <c r="N108" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="U108" s="23">
+        <v>199</v>
+      </c>
       <c r="W108" s="1" t="s">
         <v>3</v>
       </c>
@@ -6878,7 +6913,9 @@
       <c r="N109" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U109" s="28"/>
+      <c r="U109" s="23">
+        <v>89</v>
+      </c>
       <c r="W109" s="1" t="s">
         <v>4</v>
       </c>
@@ -6914,6 +6951,9 @@
       <c r="N110" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="U110" s="23">
+        <v>105</v>
+      </c>
       <c r="W110" s="1" t="s">
         <v>3</v>
       </c>
@@ -6949,7 +6989,9 @@
       <c r="N111" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U111" s="28"/>
+      <c r="U111" s="28">
+        <v>35</v>
+      </c>
       <c r="W111" s="1" t="s">
         <v>4</v>
       </c>
@@ -6985,7 +7027,9 @@
       <c r="N112" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U112" s="28"/>
+      <c r="U112" s="28">
+        <v>52</v>
+      </c>
       <c r="W112" s="1" t="s">
         <v>4</v>
       </c>
@@ -7021,14 +7065,13 @@
       <c r="N113" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U113" s="28"/>
-      <c r="W113" s="1" t="s">
-        <v>4</v>
+      <c r="U113" s="23">
+        <v>328</v>
       </c>
     </row>
     <row r="114" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A114" s="48">
-        <v>45221</v>
+        <v>45218</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>36</v>
@@ -7057,14 +7100,13 @@
       <c r="N114" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U114" s="28"/>
-      <c r="W114" s="1" t="s">
-        <v>4</v>
+      <c r="U114" s="23">
+        <v>345</v>
       </c>
     </row>
     <row r="115" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A115" s="48">
-        <v>45222</v>
+        <v>45221</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>36</v>
@@ -7093,8 +7135,11 @@
       <c r="N115" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="U115" s="28">
+        <v>34</v>
+      </c>
       <c r="W115" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="116" spans="1:23" x14ac:dyDescent="0.35">
@@ -7134,7 +7179,7 @@
     </row>
     <row r="117" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A117" s="48">
-        <v>45223</v>
+        <v>45222</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>36</v>
@@ -7203,8 +7248,8 @@
       </c>
     </row>
     <row r="119" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A119" s="53">
-        <v>45225</v>
+      <c r="A119" s="48">
+        <v>45223</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>36</v>
@@ -7238,8 +7283,8 @@
       </c>
     </row>
     <row r="120" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A120" s="53">
-        <v>45233</v>
+      <c r="A120" s="54">
+        <v>45225</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>36</v>
@@ -7274,7 +7319,7 @@
     </row>
     <row r="121" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A121" s="54">
-        <v>45237</v>
+        <v>45233</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>36</v>
@@ -7308,7 +7353,7 @@
       </c>
     </row>
     <row r="122" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A122" s="54">
+      <c r="A122" s="53">
         <v>45237</v>
       </c>
       <c r="E122" s="1" t="s">
@@ -7342,9 +7387,813 @@
         <v>3</v>
       </c>
     </row>
+    <row r="123" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A123" s="53">
+        <v>45237</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H123" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J123" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K123" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L123" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M123" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N123" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W123" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A124" s="53">
+        <v>45240</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H124" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J124" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K124" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L124" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M124" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N124" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="125" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A125" s="53">
+        <v>45240</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H125" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I125" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J125" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K125" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L125" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M125" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N125" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="126" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A126" s="53">
+        <v>45240</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I126" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J126" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K126" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L126" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M126" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N126" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="127" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A127" s="53">
+        <v>45242</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G127" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H127" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J127" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K127" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L127" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M127" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N127" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="128" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A128" s="53">
+        <v>45242</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J128" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K128" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L128" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M128" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N128" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A129" s="53">
+        <v>45243</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H129" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I129" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J129" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K129" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L129" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M129" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N129" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A130" s="53">
+        <v>45243</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H130" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I130" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J130" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K130" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L130" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M130" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N130" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A131" s="53">
+        <v>45245</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G131" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H131" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I131" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J131" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K131" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L131" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M131" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N131" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A132" s="53">
+        <v>45245</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H132" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I132" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J132" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K132" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L132" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M132" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N132" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A133" s="53">
+        <v>45258</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G133" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H133" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I133" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J133" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K133" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L133" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M133" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N133" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A134" s="53">
+        <v>45258</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H134" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J134" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K134" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L134" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M134" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N134" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A135" s="53">
+        <v>45259</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G135" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H135" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I135" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J135" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K135" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L135" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M135" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N135" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A136" s="53">
+        <v>45259</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G136" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H136" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J136" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K136" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L136" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M136" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N136" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A137" s="53">
+        <v>45259</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G137" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H137" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I137" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J137" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K137" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L137" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M137" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N137" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A138" s="53">
+        <v>45266</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G138" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H138" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J138" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K138" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L138" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M138" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N138" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A139" s="53">
+        <v>45266</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G139" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H139" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I139" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J139" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K139" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L139" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M139" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N139" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A140" s="53">
+        <v>45267</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H140" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I140" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J140" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K140" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L140" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M140" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N140" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A141" s="53">
+        <v>45267</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G141" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H141" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I141" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J141" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K141" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L141" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M141" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N141" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A142" s="53">
+        <v>45267</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I142" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J142" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K142" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L142" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M142" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N142" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A143" s="53"/>
+      <c r="B143" s="1" cm="1">
+        <f t="array" ref="B143:B173">_xlfn.UNIQUE(A89:A142)</f>
+        <v>45153</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A144" s="53"/>
+      <c r="B144" s="1">
+        <v>45154</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" s="53"/>
+      <c r="B145" s="1">
+        <v>45155</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146" s="53"/>
+      <c r="B146" s="1">
+        <v>45156</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" s="53"/>
+      <c r="B147" s="1">
+        <v>45165</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B148" s="1">
+        <v>45168</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B149" s="1">
+        <v>45169</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B150" s="1">
+        <v>45174</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B151" s="1">
+        <v>45175</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B152" s="1">
+        <v>45191</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B153" s="1">
+        <v>45193</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B154" s="1">
+        <v>45198</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B155" s="1">
+        <v>45204</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B156" s="1">
+        <v>45205</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B157" s="1">
+        <v>45214</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B158" s="1">
+        <v>45216</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B159" s="1">
+        <v>45218</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B160" s="1">
+        <v>45221</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B161" s="1">
+        <v>45222</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B162" s="1">
+        <v>45223</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B163" s="1">
+        <v>45225</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B164" s="1">
+        <v>45233</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B165" s="1">
+        <v>45237</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B166" s="1">
+        <v>45240</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B167" s="1">
+        <v>45242</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B168" s="1">
+        <v>45243</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B169" s="1">
+        <v>45245</v>
+      </c>
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B170" s="1">
+        <v>45258</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B171" s="1">
+        <v>45259</v>
+      </c>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B172" s="1">
+        <v>45266</v>
+      </c>
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B173" s="1">
+        <v>45267</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AC122" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}"/>
-  <conditionalFormatting sqref="AA20:AC151">
+  <autoFilter ref="A1:AC123" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}"/>
+  <conditionalFormatting sqref="AA20:AC154">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"M"</formula>
     </cfRule>
@@ -7368,13 +8217,13 @@
           <x14:formula1>
             <xm:f>Validation!$B$2:$B$23</xm:f>
           </x14:formula1>
-          <xm:sqref>E1021:E1025 D2:D1025</xm:sqref>
+          <xm:sqref>E1024:E1028 D2:D1028</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{31323E06-499B-45B5-9D6B-FA064BFCB0F6}">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1020</xm:sqref>
+          <xm:sqref>E2:E1023</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Stable version prior to adding planetmapper
Will be adding planetmapper incident and emission planes to files *after* this commit.
</commit_message>
<xml_diff>
--- a/Jupiter Session Processing and Analysis Notes.xlsx
+++ b/Jupiter Session Processing and Analysis Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA0BF08-6BD1-49FF-8CAB-064184E79B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D3B82B-63A8-4E78-B41B-9ADC0EE434A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="560" firstSheet="1" activeTab="1" xr2:uid="{05635B54-1AD3-49CD-8C06-A4005DAA2CD5}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Validation" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Database!$A$1:$AC$123</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Database!$A$1:$AC$174</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -41,30 +41,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="133">
   <si>
     <t>2020-07-20-0457_9-Jupiter-NoWV-NH3Abs656-0.9to1.1scale_MapFlattened-CM2_L360_MAP-BARE.png</t>
   </si>
@@ -583,7 +561,7 @@
     <t>Sum of Exp</t>
   </si>
   <si>
-    <t>?</t>
+    <t>MUSE</t>
   </si>
 </sst>
 </file>
@@ -741,7 +719,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -898,9 +876,6 @@
     <xf numFmtId="167" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -953,7 +928,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Steven Hill" refreshedDate="45026.557642245367" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="86" xr:uid="{FA8D1267-E257-44DD-BA0D-F8753C05025E}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:F87" sheet="Database"/>
+    <worksheetSource ref="A1:F89" sheet="Database"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="DateUT" numFmtId="167">
@@ -2745,16 +2720,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC173"/>
+  <dimension ref="A1:AC152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B85" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B143" sqref="B143:B173"/>
+      <selection pane="bottomRight" activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3789,7 +3764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="50">
         <v>44076</v>
       </c>
@@ -3804,7 +3779,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="50">
         <v>44077</v>
       </c>
@@ -3819,7 +3794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="50">
         <v>44078</v>
       </c>
@@ -3834,7 +3809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:29" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:29" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="50">
         <v>44087</v>
       </c>
@@ -3867,7 +3842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:29" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:29" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="50">
         <v>44088</v>
       </c>
@@ -3900,7 +3875,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="50">
         <v>44089</v>
       </c>
@@ -3912,7 +3887,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:29" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:29" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="50">
         <v>44098</v>
       </c>
@@ -3959,7 +3934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:29" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:29" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="50">
         <v>44099</v>
       </c>
@@ -3995,7 +3970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="50">
         <v>44111</v>
       </c>
@@ -4007,7 +3982,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="50">
         <v>44112</v>
       </c>
@@ -4019,7 +3994,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="50">
         <v>44113</v>
       </c>
@@ -4269,7 +4244,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="46">
         <v>44420</v>
       </c>
@@ -4293,7 +4268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="46">
         <v>44425</v>
       </c>
@@ -4317,7 +4292,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="46">
         <v>44438</v>
       </c>
@@ -4341,7 +4316,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="46">
         <v>44444</v>
       </c>
@@ -4367,7 +4342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="46">
         <v>44445</v>
       </c>
@@ -4890,7 +4865,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="46">
         <v>44522</v>
       </c>
@@ -4908,7 +4883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:29" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="46">
         <v>44523</v>
       </c>
@@ -5155,56 +5130,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:29" ht="29" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A66" s="47">
+        <v>44772</v>
+      </c>
+      <c r="B66" s="13"/>
+      <c r="E66" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:29" ht="29" x14ac:dyDescent="0.35">
+      <c r="A67" s="47">
         <v>44783</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I66" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J66" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K66" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="L66" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="M66" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="N66" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="T66" s="29">
-        <v>11.8</v>
-      </c>
-      <c r="U66" s="28">
-        <v>347.8</v>
-      </c>
-      <c r="V66" s="23">
-        <v>265.8</v>
-      </c>
-      <c r="W66" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="X66" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A67" s="47">
-        <v>44785</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>36</v>
@@ -5233,25 +5170,25 @@
       <c r="N67" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="T67" s="23">
-        <v>335.4</v>
-      </c>
-      <c r="U67" s="31">
-        <v>296.10000000000002</v>
+      <c r="T67" s="29">
+        <v>11.8</v>
+      </c>
+      <c r="U67" s="28">
+        <v>347.8</v>
       </c>
       <c r="V67" s="23">
-        <v>214.6</v>
+        <v>265.8</v>
       </c>
       <c r="W67" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="X67" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A68" s="47">
-        <v>44791</v>
+        <v>44785</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>36</v>
@@ -5281,63 +5218,60 @@
         <v>87</v>
       </c>
       <c r="T68" s="23">
+        <v>335.4</v>
+      </c>
+      <c r="U68" s="31">
+        <v>296.10000000000002</v>
+      </c>
+      <c r="V68" s="23">
+        <v>214.6</v>
+      </c>
+      <c r="W68" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="X68" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A69" s="47">
+        <v>44791</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J69" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K69" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L69" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M69" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N69" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="T69" s="23">
         <v>98.5</v>
       </c>
-      <c r="U68" s="28">
+      <c r="U69" s="28">
         <v>14.3</v>
       </c>
-      <c r="V68" s="23">
+      <c r="V69" s="23">
         <v>294.39999999999998</v>
-      </c>
-      <c r="W68" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="X68" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="69" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="47">
-        <v>44801</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H69" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I69" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J69" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K69" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="L69" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="M69" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="N69" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="O69" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="T69" s="23">
-        <v>186.7</v>
-      </c>
-      <c r="U69" s="28">
-        <v>26.7</v>
-      </c>
-      <c r="V69" s="23">
-        <v>309.39999999999998</v>
       </c>
       <c r="W69" s="1" t="s">
         <v>4</v>
@@ -5348,7 +5282,7 @@
     </row>
     <row r="70" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A70" s="47">
-        <v>44803</v>
+        <v>44801</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>36</v>
@@ -5381,21 +5315,24 @@
         <v>77</v>
       </c>
       <c r="T70" s="23">
-        <v>137.19999999999999</v>
-      </c>
-      <c r="U70" s="35">
-        <v>322</v>
+        <v>186.7</v>
+      </c>
+      <c r="U70" s="28">
+        <v>26.7</v>
       </c>
       <c r="V70" s="23">
-        <v>245.2</v>
+        <v>309.39999999999998</v>
       </c>
       <c r="W70" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="X70" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="71" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A71" s="47">
-        <v>44805</v>
+        <v>44803</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>36</v>
@@ -5428,24 +5365,21 @@
         <v>77</v>
       </c>
       <c r="T71" s="23">
-        <v>96.8</v>
-      </c>
-      <c r="U71" s="31">
-        <v>266.3</v>
+        <v>137.19999999999999</v>
+      </c>
+      <c r="U71" s="35">
+        <v>322</v>
       </c>
       <c r="V71" s="23">
-        <v>190.1</v>
+        <v>245.2</v>
       </c>
       <c r="W71" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="X71" s="7" t="s">
-        <v>125</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A72" s="47">
-        <v>44808</v>
+        <v>44805</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>36</v>
@@ -5477,22 +5411,25 @@
       <c r="O72" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="T72" s="30">
-        <v>231.2</v>
-      </c>
-      <c r="U72" s="28">
-        <v>17.600000000000001</v>
+      <c r="T72" s="23">
+        <v>96.8</v>
+      </c>
+      <c r="U72" s="31">
+        <v>266.3</v>
       </c>
       <c r="V72" s="23">
-        <v>302.2</v>
+        <v>190.1</v>
       </c>
       <c r="W72" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="X72" s="7" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="73" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A73" s="47">
-        <v>44809</v>
+        <v>44808</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>36</v>
@@ -5524,61 +5461,61 @@
       <c r="O73" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="T73" s="29">
+      <c r="T73" s="30">
+        <v>231.2</v>
+      </c>
+      <c r="U73" s="28">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="V73" s="23">
+        <v>302.2</v>
+      </c>
+      <c r="W73" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="47">
+        <v>44809</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K74" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L74" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="M74" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N74" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="O74" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="T74" s="29">
         <v>5.4</v>
       </c>
-      <c r="U73" s="32">
+      <c r="U74" s="32">
         <v>144.4</v>
       </c>
-      <c r="V73" s="23">
+      <c r="V74" s="23">
         <v>69.2</v>
-      </c>
-      <c r="W73" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="X73" s="33" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A74" s="47">
-        <v>44816</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H74" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I74" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J74" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K74" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="L74" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="M74" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="N74" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="T74" s="29">
-        <v>16</v>
-      </c>
-      <c r="U74" s="23">
-        <v>101.7</v>
-      </c>
-      <c r="V74" s="23">
-        <v>28.4</v>
       </c>
       <c r="W74" s="1" t="s">
         <v>3</v>
@@ -5589,7 +5526,7 @@
     </row>
     <row r="75" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A75" s="47">
-        <v>44817</v>
+        <v>44816</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>36</v>
@@ -5618,25 +5555,25 @@
       <c r="N75" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="T75" s="23">
-        <v>152.1</v>
-      </c>
-      <c r="U75" s="31">
-        <v>230.3</v>
+      <c r="T75" s="29">
+        <v>16</v>
+      </c>
+      <c r="U75" s="23">
+        <v>101.7</v>
       </c>
       <c r="V75" s="23">
-        <v>157.30000000000001</v>
+        <v>28.4</v>
       </c>
       <c r="W75" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="X75" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="76" spans="1:29" ht="29" x14ac:dyDescent="0.35">
+      <c r="X75" s="33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="76" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A76" s="47">
-        <v>44823</v>
+        <v>44817</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>36</v>
@@ -5665,28 +5602,28 @@
       <c r="N76" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="T76" s="29">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="U76" s="28">
-        <v>50.4</v>
+      <c r="T76" s="23">
+        <v>152.1</v>
+      </c>
+      <c r="U76" s="31">
+        <v>230.3</v>
       </c>
       <c r="V76" s="23">
-        <v>339</v>
+        <v>157.30000000000001</v>
       </c>
       <c r="W76" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="X76" s="2" t="s">
-        <v>118</v>
+        <v>3</v>
+      </c>
+      <c r="X76" s="7" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="77" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A77" s="47">
-        <v>44829</v>
+        <v>44823</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>36</v>
+        <v>132</v>
       </c>
       <c r="G77" s="3" t="s">
         <v>86</v>
@@ -5712,25 +5649,12 @@
       <c r="N77" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="T77" s="23">
-        <v>296.2</v>
-      </c>
-      <c r="U77" s="31">
-        <v>282.5</v>
-      </c>
-      <c r="V77" s="23">
-        <v>212.7</v>
-      </c>
-      <c r="W77" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="X77" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="T77" s="29"/>
+      <c r="U77" s="28"/>
+    </row>
+    <row r="78" spans="1:29" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="47">
-        <v>44843</v>
+        <v>44823</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>36</v>
@@ -5759,42 +5683,72 @@
       <c r="N78" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="T78" s="23">
-        <v>317.3</v>
-      </c>
-      <c r="U78" s="27">
-        <v>197.1</v>
+      <c r="T78" s="29">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="U78" s="28">
+        <v>50.4</v>
       </c>
       <c r="V78" s="23">
-        <v>131</v>
+        <v>339</v>
       </c>
       <c r="W78" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="X78" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="79" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A79" s="47">
-        <v>44843</v>
+        <v>44829</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I79" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K79" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L79" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M79" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N79" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="T79" s="23">
-        <v>267</v>
-      </c>
-      <c r="U79" s="32">
-        <v>147</v>
+        <v>296.2</v>
+      </c>
+      <c r="U79" s="31">
+        <v>282.5</v>
       </c>
       <c r="V79" s="23">
-        <v>81</v>
+        <v>212.7</v>
+      </c>
+      <c r="W79" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="X79" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="80" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A80" s="47">
-        <v>44847</v>
+        <v>44843</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>36</v>
@@ -5824,68 +5778,44 @@
         <v>87</v>
       </c>
       <c r="T80" s="23">
-        <v>168.9</v>
-      </c>
-      <c r="U80" s="28">
-        <v>18.7</v>
+        <v>317.3</v>
+      </c>
+      <c r="U80" s="27">
+        <v>197.1</v>
       </c>
       <c r="V80" s="23">
-        <v>313.60000000000002</v>
+        <v>131</v>
       </c>
       <c r="W80" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="X80" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A81" s="47">
-        <v>44853</v>
+        <v>44843</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G81" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H81" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I81" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J81" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K81" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="L81" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="M81" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="N81" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="T81" s="29">
-        <v>34.9</v>
-      </c>
-      <c r="U81" s="27">
-        <v>198.9</v>
+      <c r="T81" s="23">
+        <v>267</v>
+      </c>
+      <c r="U81" s="32">
+        <v>147</v>
       </c>
       <c r="V81" s="23">
-        <v>135.4</v>
-      </c>
-      <c r="W81" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="X81" s="33" t="s">
-        <v>121</v>
+        <v>81</v>
+      </c>
+      <c r="X81" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A82" s="47">
-        <v>44854</v>
+        <v>44847</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>36</v>
@@ -5914,14 +5844,14 @@
       <c r="N82" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="T82" s="36">
-        <v>228</v>
-      </c>
-      <c r="U82" s="37">
-        <v>24.1</v>
-      </c>
-      <c r="V82" s="38">
-        <v>320.89999999999998</v>
+      <c r="T82" s="23">
+        <v>168.9</v>
+      </c>
+      <c r="U82" s="28">
+        <v>18.7</v>
+      </c>
+      <c r="V82" s="23">
+        <v>313.60000000000002</v>
       </c>
       <c r="W82" s="1" t="s">
         <v>4</v>
@@ -5929,7 +5859,7 @@
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A83" s="47">
-        <v>44855</v>
+        <v>44853</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>36</v>
@@ -5958,28 +5888,28 @@
       <c r="N83" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="T83" s="39">
-        <v>0.3</v>
-      </c>
-      <c r="U83" s="40">
-        <v>149</v>
-      </c>
-      <c r="V83" s="38">
-        <v>86.1</v>
+      <c r="T83" s="29">
+        <v>34.9</v>
+      </c>
+      <c r="U83" s="27">
+        <v>198.9</v>
+      </c>
+      <c r="V83" s="23">
+        <v>135.4</v>
       </c>
       <c r="W83" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="X83" s="34" t="s">
-        <v>117</v>
+        <v>3</v>
+      </c>
+      <c r="X83" s="33" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A84" s="47">
-        <v>44865</v>
+        <v>44854</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G84" s="3" t="s">
         <v>86</v>
@@ -5997,18 +5927,33 @@
         <v>87</v>
       </c>
       <c r="L84" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="X84" s="2" t="s">
-        <v>80</v>
+        <v>112</v>
+      </c>
+      <c r="M84" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N84" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="T84" s="36">
+        <v>228</v>
+      </c>
+      <c r="U84" s="37">
+        <v>24.1</v>
+      </c>
+      <c r="V84" s="38">
+        <v>320.89999999999998</v>
+      </c>
+      <c r="W84" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A85" s="47">
-        <v>44866</v>
+        <v>44855</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G85" s="3" t="s">
         <v>86</v>
@@ -6026,15 +5971,33 @@
         <v>87</v>
       </c>
       <c r="L85" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="X85" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+      <c r="M85" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N85" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="T85" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="U85" s="40">
+        <v>149</v>
+      </c>
+      <c r="V85" s="38">
+        <v>86.1</v>
+      </c>
+      <c r="W85" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X85" s="34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="47">
-        <v>44874</v>
+        <v>44865</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>37</v>
@@ -6061,9 +6024,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:24" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="47">
-        <v>44886</v>
+        <v>44866</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>37</v>
@@ -6086,86 +6049,68 @@
       <c r="L87" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="X87" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="88" spans="1:24" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="47">
+        <v>44874</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K88" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L88" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="X88" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="89" spans="1:24" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="47">
+        <v>44886</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K89" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L89" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A90" s="47">
         <v>44939</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H88" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I88" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J88" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K88" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="L88" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="M88" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="N88" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="U88" s="28">
-        <v>47.5</v>
-      </c>
-      <c r="W88" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A89" s="48">
-        <v>45153</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I89" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J89" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K89" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="L89" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="M89" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="N89" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="U89" s="51">
-        <v>145</v>
-      </c>
-      <c r="W89" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A90" s="48">
-        <v>45153</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>36</v>
@@ -6194,13 +6139,16 @@
       <c r="N90" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U90" s="23" t="s">
-        <v>132</v>
+      <c r="U90" s="28">
+        <v>47.5</v>
+      </c>
+      <c r="W90" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A91" s="48">
-        <v>45154</v>
+        <v>45153</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>36</v>
@@ -6229,8 +6177,8 @@
       <c r="N91" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U91" s="29">
-        <v>306</v>
+      <c r="U91" s="51">
+        <v>145</v>
       </c>
       <c r="W91" s="1" t="s">
         <v>3</v>
@@ -6238,7 +6186,7 @@
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A92" s="48">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>36</v>
@@ -6267,8 +6215,8 @@
       <c r="N92" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U92" s="52">
-        <v>91</v>
+      <c r="U92" s="29">
+        <v>306</v>
       </c>
       <c r="W92" s="1" t="s">
         <v>3</v>
@@ -6276,7 +6224,7 @@
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A93" s="48">
-        <v>45156</v>
+        <v>45155</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>36</v>
@@ -6305,8 +6253,8 @@
       <c r="N93" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U93" s="31">
-        <v>250</v>
+      <c r="U93" s="52">
+        <v>91</v>
       </c>
       <c r="W93" s="1" t="s">
         <v>3</v>
@@ -6314,7 +6262,7 @@
     </row>
     <row r="94" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A94" s="48">
-        <v>45165</v>
+        <v>45156</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>36</v>
@@ -6343,8 +6291,8 @@
       <c r="N94" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U94" s="51">
-        <v>159</v>
+      <c r="U94" s="31">
+        <v>250</v>
       </c>
       <c r="W94" s="1" t="s">
         <v>3</v>
@@ -6382,7 +6330,7 @@
         <v>87</v>
       </c>
       <c r="U95" s="51">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="W95" s="1" t="s">
         <v>3</v>
@@ -6390,7 +6338,7 @@
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A96" s="48">
-        <v>45168</v>
+        <v>45165</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>36</v>
@@ -6419,8 +6367,8 @@
       <c r="N96" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U96" s="31">
-        <v>258</v>
+      <c r="U96" s="51">
+        <v>173</v>
       </c>
       <c r="W96" s="1" t="s">
         <v>3</v>
@@ -6428,7 +6376,7 @@
     </row>
     <row r="97" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A97" s="48">
-        <v>45169</v>
+        <v>45168</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>36</v>
@@ -6457,11 +6405,11 @@
       <c r="N97" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U97" s="28">
-        <v>40</v>
+      <c r="U97" s="31">
+        <v>258</v>
       </c>
       <c r="W97" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:23" x14ac:dyDescent="0.35">
@@ -6496,7 +6444,7 @@
         <v>87</v>
       </c>
       <c r="U98" s="28">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="W98" s="1" t="s">
         <v>4</v>
@@ -6504,7 +6452,7 @@
     </row>
     <row r="99" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A99" s="48">
-        <v>45174</v>
+        <v>45169</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>36</v>
@@ -6534,7 +6482,7 @@
         <v>87</v>
       </c>
       <c r="U99" s="28">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="W99" s="1" t="s">
         <v>4</v>
@@ -6571,16 +6519,16 @@
       <c r="N100" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U100" s="52">
-        <v>93</v>
+      <c r="U100" s="28">
+        <v>77</v>
       </c>
       <c r="W100" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A101" s="48">
-        <v>45175</v>
+        <v>45174</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>36</v>
@@ -6609,8 +6557,8 @@
       <c r="N101" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U101" s="31">
-        <v>224</v>
+      <c r="U101" s="52">
+        <v>93</v>
       </c>
       <c r="W101" s="1" t="s">
         <v>3</v>
@@ -6648,7 +6596,7 @@
         <v>87</v>
       </c>
       <c r="U102" s="31">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="W102" s="1" t="s">
         <v>3</v>
@@ -6656,7 +6604,7 @@
     </row>
     <row r="103" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A103" s="48">
-        <v>45191</v>
+        <v>45175</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>36</v>
@@ -6685,8 +6633,8 @@
       <c r="N103" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U103" s="29">
-        <v>286</v>
+      <c r="U103" s="31">
+        <v>242</v>
       </c>
       <c r="W103" s="1" t="s">
         <v>3</v>
@@ -6694,7 +6642,7 @@
     </row>
     <row r="104" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A104" s="48">
-        <v>45193</v>
+        <v>45191</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>36</v>
@@ -6723,16 +6671,16 @@
       <c r="N104" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U104" s="28">
-        <v>60</v>
+      <c r="U104" s="29">
+        <v>286</v>
       </c>
       <c r="W104" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A105" s="48">
-        <v>45198</v>
+        <v>45193</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>36</v>
@@ -6761,16 +6709,16 @@
       <c r="N105" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U105" s="23">
-        <v>224</v>
+      <c r="U105" s="28">
+        <v>60</v>
       </c>
       <c r="W105" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A106" s="48">
-        <v>45204</v>
+        <v>45198</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>36</v>
@@ -6799,16 +6747,16 @@
       <c r="N106" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U106" s="28">
-        <v>27</v>
+      <c r="U106" s="23">
+        <v>224</v>
       </c>
       <c r="W106" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A107" s="48">
-        <v>45205</v>
+        <v>45204</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>36</v>
@@ -6837,11 +6785,11 @@
       <c r="N107" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U107" s="23">
-        <v>180</v>
+      <c r="U107" s="28">
+        <v>27</v>
       </c>
       <c r="W107" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108" spans="1:23" x14ac:dyDescent="0.35">
@@ -6876,7 +6824,7 @@
         <v>87</v>
       </c>
       <c r="U108" s="23">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="W108" s="1" t="s">
         <v>3</v>
@@ -6884,7 +6832,7 @@
     </row>
     <row r="109" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A109" s="48">
-        <v>45214</v>
+        <v>45205</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>36</v>
@@ -6914,10 +6862,10 @@
         <v>87</v>
       </c>
       <c r="U109" s="23">
-        <v>89</v>
+        <v>199</v>
       </c>
       <c r="W109" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:23" x14ac:dyDescent="0.35">
@@ -6952,15 +6900,15 @@
         <v>87</v>
       </c>
       <c r="U110" s="23">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="W110" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A111" s="48">
-        <v>45216</v>
+        <v>45214</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>36</v>
@@ -6989,11 +6937,11 @@
       <c r="N111" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U111" s="28">
-        <v>35</v>
+      <c r="U111" s="23">
+        <v>105</v>
       </c>
       <c r="W111" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112" spans="1:23" x14ac:dyDescent="0.35">
@@ -7028,7 +6976,7 @@
         <v>87</v>
       </c>
       <c r="U112" s="28">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="W112" s="1" t="s">
         <v>4</v>
@@ -7036,7 +6984,7 @@
     </row>
     <row r="113" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A113" s="48">
-        <v>45218</v>
+        <v>45216</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>36</v>
@@ -7065,8 +7013,11 @@
       <c r="N113" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U113" s="23">
-        <v>328</v>
+      <c r="U113" s="28">
+        <v>52</v>
+      </c>
+      <c r="W113" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="114" spans="1:23" x14ac:dyDescent="0.35">
@@ -7101,12 +7052,12 @@
         <v>87</v>
       </c>
       <c r="U114" s="23">
-        <v>345</v>
+        <v>328</v>
       </c>
     </row>
     <row r="115" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A115" s="48">
-        <v>45221</v>
+        <v>45218</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>36</v>
@@ -7135,16 +7086,13 @@
       <c r="N115" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U115" s="28">
-        <v>34</v>
-      </c>
-      <c r="W115" s="1" t="s">
-        <v>4</v>
+      <c r="U115" s="23">
+        <v>345</v>
       </c>
     </row>
     <row r="116" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A116" s="48">
-        <v>45222</v>
+        <v>45221</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>36</v>
@@ -7173,8 +7121,11 @@
       <c r="N116" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="U116" s="28">
+        <v>34</v>
+      </c>
       <c r="W116" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:23" x14ac:dyDescent="0.35">
@@ -7214,7 +7165,7 @@
     </row>
     <row r="118" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A118" s="48">
-        <v>45223</v>
+        <v>45222</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>36</v>
@@ -7283,8 +7234,8 @@
       </c>
     </row>
     <row r="120" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A120" s="54">
-        <v>45225</v>
+      <c r="A120" s="48">
+        <v>45223</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>36</v>
@@ -7318,8 +7269,8 @@
       </c>
     </row>
     <row r="121" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A121" s="54">
-        <v>45233</v>
+      <c r="A121" s="48">
+        <v>45225</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>36</v>
@@ -7353,8 +7304,8 @@
       </c>
     </row>
     <row r="122" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A122" s="53">
-        <v>45237</v>
+      <c r="A122" s="48">
+        <v>45233</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>36</v>
@@ -7424,7 +7375,7 @@
     </row>
     <row r="124" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A124" s="53">
-        <v>45240</v>
+        <v>45237</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>36</v>
@@ -7452,6 +7403,9 @@
       </c>
       <c r="N124" s="3" t="s">
         <v>87</v>
+      </c>
+      <c r="W124" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="125" spans="1:23" x14ac:dyDescent="0.35">
@@ -7520,7 +7474,7 @@
     </row>
     <row r="127" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A127" s="53">
-        <v>45242</v>
+        <v>45240</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>36</v>
@@ -7584,7 +7538,7 @@
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A129" s="53">
-        <v>45243</v>
+        <v>45242</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>36</v>
@@ -7648,7 +7602,7 @@
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A131" s="53">
-        <v>45245</v>
+        <v>45243</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>36</v>
@@ -7712,7 +7666,7 @@
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A133" s="53">
-        <v>45258</v>
+        <v>45245</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>36</v>
@@ -7776,7 +7730,7 @@
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A135" s="53">
-        <v>45259</v>
+        <v>45258</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>36</v>
@@ -7872,7 +7826,7 @@
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A138" s="53">
-        <v>45266</v>
+        <v>45259</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>36</v>
@@ -7936,7 +7890,7 @@
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A140" s="53">
-        <v>45267</v>
+        <v>45266</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>36</v>
@@ -8031,169 +7985,335 @@
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A143" s="53"/>
-      <c r="B143" s="1" cm="1">
-        <f t="array" ref="B143:B173">_xlfn.UNIQUE(A89:A142)</f>
-        <v>45153</v>
+      <c r="A143" s="53">
+        <v>45267</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G143" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H143" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I143" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J143" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K143" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L143" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M143" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N143" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A144" s="53"/>
-      <c r="B144" s="1">
-        <v>45154</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A145" s="53"/>
-      <c r="B145" s="1">
-        <v>45155</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A146" s="53"/>
-      <c r="B146" s="1">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A147" s="53"/>
-      <c r="B147" s="1">
-        <v>45165</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B148" s="1">
-        <v>45168</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B149" s="1">
-        <v>45169</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B150" s="1">
-        <v>45174</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B151" s="1">
-        <v>45175</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B152" s="1">
-        <v>45191</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B153" s="1">
-        <v>45193</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B154" s="1">
-        <v>45198</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B155" s="1">
-        <v>45204</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B156" s="1">
-        <v>45205</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B157" s="1">
-        <v>45214</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B158" s="1">
-        <v>45216</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B159" s="1">
-        <v>45218</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B160" s="1">
-        <v>45221</v>
-      </c>
-    </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B161" s="1">
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B162" s="1">
-        <v>45223</v>
-      </c>
-    </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B163" s="1">
-        <v>45225</v>
-      </c>
-    </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B164" s="1">
-        <v>45233</v>
-      </c>
-    </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B165" s="1">
-        <v>45237</v>
-      </c>
-    </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B166" s="1">
-        <v>45240</v>
-      </c>
-    </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B167" s="1">
-        <v>45242</v>
-      </c>
-    </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B168" s="1">
-        <v>45243</v>
-      </c>
-    </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B169" s="1">
-        <v>45245</v>
-      </c>
-    </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B170" s="1">
-        <v>45258</v>
-      </c>
-    </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B171" s="1">
-        <v>45259</v>
-      </c>
-    </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B172" s="1">
-        <v>45266</v>
-      </c>
-    </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B173" s="1">
-        <v>45267</v>
+      <c r="A144" s="53">
+        <v>45277</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G144" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H144" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I144" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J144" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K144" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L144" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M144" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N144" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A145" s="53">
+        <v>45277</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G145" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H145" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I145" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J145" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K145" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L145" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M145" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N145" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A146" s="53">
+        <v>45277</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G146" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H146" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I146" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J146" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K146" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L146" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M146" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N146" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A147" s="53">
+        <v>45278</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G147" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H147" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I147" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J147" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K147" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L147" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M147" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N147" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A148" s="53">
+        <v>45278</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G148" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H148" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I148" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J148" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K148" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L148" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M148" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N148" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A149" s="53">
+        <v>45278</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G149" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H149" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I149" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J149" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K149" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L149" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M149" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N149" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A150" s="53">
+        <v>45278</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H150" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I150" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J150" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K150" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L150" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M150" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N150" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A151" s="53">
+        <v>45278</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G151" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H151" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I151" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J151" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K151" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L151" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M151" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N151" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A152" s="53">
+        <v>45278</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G152" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H152" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I152" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J152" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K152" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L152" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M152" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N152" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC123" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}"/>
-  <conditionalFormatting sqref="AA20:AC154">
+  <autoFilter ref="A1:AC174" xr:uid="{7C3155B5-1B77-468F-93F8-11D564BBF4E2}">
+    <filterColumn colId="4">
+      <filters blank="1">
+        <filter val="CMOS"/>
+        <filter val="MUSE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="AA20:AC155">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"M"</formula>
     </cfRule>
@@ -8212,18 +8332,24 @@
   <pageSetup scale="36" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{33D43DC1-A51A-45A6-9175-025FA7461CC7}">
           <x14:formula1>
             <xm:f>Validation!$B$2:$B$23</xm:f>
           </x14:formula1>
-          <xm:sqref>E1024:E1028 D2:D1028</xm:sqref>
+          <xm:sqref>E1025:E1029 D2:D1029</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{31323E06-499B-45B5-9D6B-FA064BFCB0F6}">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1023</xm:sqref>
+          <xm:sqref>E175:E1024</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{52CBD5CB-8ADC-4E52-86AF-74FDF3C7F82D}">
+          <x14:formula1>
+            <xm:f>Validation!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E174</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8235,8 +8361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90829B0-B3A3-41EC-85F6-16D16F9F4A42}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B2:B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8266,6 +8392,9 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
       <c r="B4" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Temp Local for NEZ Analysis
Committing a local copy of a working version of the NEZ analysis tool before attempting to fix the Dark Proj aspect of the code
</commit_message>
<xml_diff>
--- a/Jupiter Session Processing and Analysis Notes.xlsx
+++ b/Jupiter Session Processing and Analysis Notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D3B82B-63A8-4E78-B41B-9ADC0EE434A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8F2352-8C0B-4704-BDB1-D15480A4AC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="560" firstSheet="1" activeTab="1" xr2:uid="{05635B54-1AD3-49CD-8C06-A4005DAA2CD5}"/>
   </bookViews>
@@ -24,6 +24,7 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="133">
   <si>
     <t>2020-07-20-0457_9-Jupiter-NoWV-NH3Abs656-0.9to1.1scale_MapFlattened-CM2_L360_MAP-BARE.png</t>
   </si>
@@ -2027,9 +2028,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2067,7 +2068,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2173,7 +2174,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2315,7 +2316,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2723,18 +2724,18 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC152"/>
+  <dimension ref="A1:AC155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B85" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B135" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C99" sqref="C99"/>
+      <selection pane="bottomRight" activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" style="45" customWidth="1"/>
+    <col min="1" max="1" width="14" style="45" customWidth="1"/>
     <col min="2" max="2" width="10.453125" style="1" customWidth="1"/>
     <col min="3" max="3" width="46.54296875" style="3" customWidth="1"/>
     <col min="4" max="4" width="13" style="4" customWidth="1"/>
@@ -8301,6 +8302,102 @@
         <v>87</v>
       </c>
       <c r="N152" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A153" s="53">
+        <v>45289</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G153" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H153" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I153" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J153" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K153" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L153" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M153" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N153" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A154" s="53">
+        <v>45289</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H154" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I154" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J154" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K154" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L154" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M154" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N154" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A155" s="53">
+        <v>45289</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G155" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H155" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I155" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J155" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K155" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L155" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M155" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N155" s="3" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>